<commit_message>
Made some changes on the data masking logic
</commit_message>
<xml_diff>
--- a/backend/uploads/masked/masked_Student_Information.xlsx
+++ b/backend/uploads/masked/masked_Student_Information.xlsx
@@ -517,7 +517,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Ali bin Ahmad</t>
+          <t>A***********d</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -535,7 +535,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>012-3456789</t>
+          <t>0*********9</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -545,7 +545,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>ali.ahmad@example.com</t>
+          <t>a*******d@example.com</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -586,7 +586,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Siti binti Aminah</t>
+          <t>S***************h</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -604,7 +604,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>013-4567890</t>
+          <t>0*********0</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -614,7 +614,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>siti.aminah@example.com</t>
+          <t>s*********h@example.com</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -655,7 +655,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Lim Wei Chong</t>
+          <t>L***********g</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -673,7 +673,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>014-5678901</t>
+          <t>0*********1</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -683,7 +683,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>lim.weichong@example.com</t>
+          <t>l**********g@example.com</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -724,7 +724,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Preeti Kaur</t>
+          <t>P*********r</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -742,7 +742,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>015-6789012</t>
+          <t>0*********2</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -752,7 +752,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>preeti.kaur@example.com</t>
+          <t>p*********r@example.com</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -793,7 +793,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Muhammad Hafiz</t>
+          <t>M************z</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -811,7 +811,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>016-7890123</t>
+          <t>0*********3</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -821,7 +821,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>muhammad.hafiz@example.com</t>
+          <t>m************z@example.com</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -862,7 +862,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Chong Mei Ling</t>
+          <t>C************g</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -880,7 +880,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>017-8901234</t>
+          <t>0*********4</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -890,7 +890,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>chong.mei@example.com</t>
+          <t>c*******i@example.com</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -931,7 +931,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Arun Raj</t>
+          <t>A******j</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -949,7 +949,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>018-9012345</t>
+          <t>0*********5</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -959,7 +959,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>arun.raj@example.com</t>
+          <t>a******j@example.com</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -1000,7 +1000,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Farah binti Zain</t>
+          <t>F**************n</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1018,7 +1018,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>019-0123456</t>
+          <t>0*********6</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1028,7 +1028,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>farah.zain@example.com</t>
+          <t>f********n@example.com</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -1069,7 +1069,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Tan Ah Heng</t>
+          <t>T*********g</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1087,7 +1087,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>010-2345678</t>
+          <t>0*********8</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1097,7 +1097,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>tan.ahheng@example.com</t>
+          <t>t********g@example.com</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -1138,7 +1138,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Anusha Devi</t>
+          <t>A*********i</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1156,7 +1156,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>011-3456789</t>
+          <t>0*********9</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1166,7 +1166,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>anusha.devi@example.com</t>
+          <t>a*********i@example.com</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -1207,7 +1207,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Nur Aisyah</t>
+          <t>N********h</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1225,7 +1225,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>012-5678901</t>
+          <t>0*********1</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1235,7 +1235,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>nur.aisyah@example.com</t>
+          <t>n********h@example.com</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -1276,7 +1276,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Wong Siew Mei</t>
+          <t>W***********i</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1294,7 +1294,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>013-6789012</t>
+          <t>0*********2</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1304,7 +1304,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>wong.siewmei@example.com</t>
+          <t>w**********i@example.com</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -1345,7 +1345,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Thiru Selvan</t>
+          <t>T**********n</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1363,7 +1363,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>014-7890123</t>
+          <t>0*********3</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1373,7 +1373,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>thiru.selvan@example.com</t>
+          <t>t**********n@example.com</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -1414,7 +1414,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Aina binti Razak</t>
+          <t>A**************k</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1432,7 +1432,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>015-8901234</t>
+          <t>0*********4</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1442,7 +1442,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>aina.razak@example.com</t>
+          <t>a********k@example.com</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -1483,7 +1483,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Yong Kai Wen</t>
+          <t>Y**********n</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1501,7 +1501,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>016-9012345</t>
+          <t>0*********5</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1511,7 +1511,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>yong.kaiwen@example.com</t>
+          <t>y*********n@example.com</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -1552,7 +1552,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Hema Latha</t>
+          <t>H********a</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1570,7 +1570,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>017-0123456</t>
+          <t>0*********6</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1580,7 +1580,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>hema.latha@example.com</t>
+          <t>h********a@example.com</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -1621,7 +1621,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Ahmad bin Abu</t>
+          <t>A***********u</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1639,7 +1639,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>018-1234567</t>
+          <t>0*********7</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1649,7 +1649,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>ahmad.abu@example.com</t>
+          <t>a*******u@example.com</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -1690,7 +1690,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Mei Fong</t>
+          <t>M******g</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1708,7 +1708,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>019-2345678</t>
+          <t>0*********8</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1718,7 +1718,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>mei.fong@example.com</t>
+          <t>m******g@example.com</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -1759,7 +1759,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Raju Kumar</t>
+          <t>R********r</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1777,7 +1777,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>010-3456789</t>
+          <t>0*********9</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1787,7 +1787,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>raju.kumar@example.com</t>
+          <t>r********r@example.com</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -1828,7 +1828,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Zainal Abidin</t>
+          <t>Z***********n</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1846,7 +1846,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>011-4567890</t>
+          <t>0*********0</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1856,7 +1856,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>zainal.abidin@example.com</t>
+          <t>z***********n@example.com</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -1897,7 +1897,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Amira binti Latif</t>
+          <t>A***************f</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1915,7 +1915,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>012-5678901</t>
+          <t>0*********1</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1925,7 +1925,7 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>amira.latif@example.com</t>
+          <t>a*********f@example.com</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -1966,7 +1966,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Chia Wei Han</t>
+          <t>C**********n</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1984,7 +1984,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>013-6789012</t>
+          <t>0*********2</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1994,7 +1994,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>chia.weihan@example.com</t>
+          <t>c*********n@example.com</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -2035,7 +2035,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Suresh Kumar</t>
+          <t>S**********r</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -2053,7 +2053,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>014-7890123</t>
+          <t>0*********3</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2063,7 +2063,7 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>suresh.kumar@example.com</t>
+          <t>s**********r@example.com</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -2104,7 +2104,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Norhidayah</t>
+          <t>N********h</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -2122,7 +2122,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>015-8901234</t>
+          <t>0*********4</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2132,7 +2132,7 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>norhidayah@example.com</t>
+          <t>n********h@example.com</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
@@ -2173,7 +2173,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Lim Wei Hui</t>
+          <t>L*********i</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -2191,7 +2191,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>016-9012345</t>
+          <t>0*********5</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2201,7 +2201,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>lim.weihui@example.com</t>
+          <t>l********i@example.com</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -2242,7 +2242,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Arvind Raj</t>
+          <t>A********j</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -2260,7 +2260,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>017-0123456</t>
+          <t>0*********6</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2270,7 +2270,7 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>arvind.raj@example.com</t>
+          <t>a********j@example.com</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
@@ -2311,7 +2311,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Safia binti Noor</t>
+          <t>S**************r</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -2329,7 +2329,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>018-1234567</t>
+          <t>0*********7</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2339,7 +2339,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>safia.noor@example.com</t>
+          <t>s********r@example.com</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
@@ -2380,7 +2380,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Wong Kin Fai</t>
+          <t>W**********i</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -2398,7 +2398,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>019-2345678</t>
+          <t>0*********8</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2408,7 +2408,7 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>wong.kinfai@example.com</t>
+          <t>w*********i@example.com</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
@@ -2449,7 +2449,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Aina binti Osman</t>
+          <t>A**************n</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -2467,7 +2467,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>010-3456789</t>
+          <t>0*********9</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2477,7 +2477,7 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>aina.osman@example.com</t>
+          <t>a********n@example.com</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
@@ -2518,7 +2518,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Kumar Narayanan</t>
+          <t>K*************n</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -2536,7 +2536,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>011-4567890</t>
+          <t>0*********0</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2546,7 +2546,7 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>kumar.narayanan@example.com</t>
+          <t>k*************n@example.com</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">

</xml_diff>

<commit_message>
Updated the data masking logic
</commit_message>
<xml_diff>
--- a/backend/uploads/masked/masked_Student_Information.xlsx
+++ b/backend/uploads/masked/masked_Student_Information.xlsx
@@ -517,7 +517,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>A***********d</t>
+          <t>Omar Moore</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -530,7 +530,8 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>123, Jalan Bukit, Kuala Lumpur</t>
+          <t>255 Sheila Forks
+Port Lisa, MT 30599</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -586,7 +587,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>S***************h</t>
+          <t>Courtney Lopez</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -599,7 +600,8 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>45, Jalan Mawar, Johor Bahru</t>
+          <t>88657 Bridges Ridges Suite 908
+New James, FM 12406</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -655,7 +657,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>L***********g</t>
+          <t>April Acevedo</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -668,7 +670,8 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>67, Jalan Kenanga, Penang</t>
+          <t>5782 Karen Freeway Apt. 121
+East Michael, MN 93036</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -724,7 +727,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>P*********r</t>
+          <t>Larry Fitzgerald</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -737,7 +740,8 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>89, Jalan Teratai, Ipoh</t>
+          <t>05018 Jonathan Causeway Suite 007
+Robertberg, PA 76718</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -793,7 +797,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>M************z</t>
+          <t>Julia Turner</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -806,7 +810,8 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>101, Jalan Dahlia, Shah Alam</t>
+          <t>557 Deborah Stravenue Suite 512
+Hunterland, PR 10743</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -862,7 +867,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>C************g</t>
+          <t>Eric Gibbs</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -875,7 +880,8 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>123, Jalan Melati, Melaka</t>
+          <t>42438 Choi Hill
+Anthonyfurt, AL 77481</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -931,7 +937,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>A******j</t>
+          <t>Shannon Chen MD</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -944,7 +950,8 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>145, Jalan Mawar, Seremban</t>
+          <t>7581 Ricky Ville Suite 054
+Edwardstown, CA 70682</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -1000,7 +1007,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>F**************n</t>
+          <t>Jeffrey Dean</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1013,7 +1020,8 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>167, Jalan Cempaka, Kuantan</t>
+          <t>50067 Jennifer Keys Apt. 550
+Ryanfort, MA 75532</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -1069,7 +1077,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>T*********g</t>
+          <t>Rebecca Mcdaniel</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1082,7 +1090,8 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>189, Jalan Anggerik, Kota Kinabalu</t>
+          <t>313 Ronald Throughway Suite 824
+Dennisside, OR 95517</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -1138,7 +1147,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>A*********i</t>
+          <t>Keith Browning</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1151,7 +1160,8 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>201, Jalan Ros, Kuala Terengganu</t>
+          <t>4141 Reed Village Apt. 499
+Brianbury, SD 77602</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -1207,7 +1217,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>N********h</t>
+          <t>Laura Sanders</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1220,7 +1230,8 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>223, Jalan Tunku, Alor Setar</t>
+          <t>PSC 1945, Box 0739
+APO AA 83783</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -1276,7 +1287,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>W***********i</t>
+          <t>Rachel Perry</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1289,7 +1300,8 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>245, Jalan Taman, Miri</t>
+          <t>19535 Joel Village
+Brownside, WV 45373</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -1345,7 +1357,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>T**********n</t>
+          <t>Thomas Ray</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1358,7 +1370,8 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>267, Jalan Desa, Kuching</t>
+          <t>154 Sonia Loaf
+Lake Danieltown, IA 33784</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1414,7 +1427,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>A**************k</t>
+          <t>Lisa Jensen</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1427,7 +1440,8 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>289, Jalan Seri, Klang</t>
+          <t>69188 Thomas Centers
+East Kimberlychester, VI 29574</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1483,7 +1497,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Y**********n</t>
+          <t>Shelby Zamora</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1496,7 +1510,8 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>301, Jalan Hijau, Georgetown</t>
+          <t>05547 Luna Crossroad
+Stonefurt, IN 30064</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1552,7 +1567,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>H********a</t>
+          <t>Amanda Tate</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1565,7 +1580,8 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>323, Jalan Biru, Kuala Lumpur</t>
+          <t>746 Brandon Locks Apt. 876
+Gabrielaville, OK 12010</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1621,7 +1637,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>A***********u</t>
+          <t>Lee Faulkner</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1634,7 +1650,8 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>345, Jalan Putih, Putrajaya</t>
+          <t>242 Martin Radial
+Greenland, DC 64953</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1690,7 +1707,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>M******g</t>
+          <t>John Patterson</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1703,7 +1720,8 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>367, Jalan Kuning, Sibu</t>
+          <t>5134 David Via
+Lake Evanbury, NV 59386</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1759,7 +1777,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>R********r</t>
+          <t>Deanna Allen</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1772,7 +1790,8 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>389, Jalan Merah, Sandakan</t>
+          <t>64830 Reyes Isle
+North Chad, PA 72164</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1828,7 +1847,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Z***********n</t>
+          <t>Wanda Ochoa</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1841,7 +1860,8 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>401, Jalan Putra, Kuala Lumpur</t>
+          <t>53668 Alisha Village
+Christopherton, MI 28909</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1897,7 +1917,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>A***************f</t>
+          <t>Hayden Patterson</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1910,7 +1930,8 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>423, Jalan Raja, Alor Setar</t>
+          <t>55868 Mary Falls Suite 905
+Kimberlyland, TX 41676</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1966,7 +1987,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>C**********n</t>
+          <t>Chris Weber</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1979,7 +2000,8 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>445, Jalan Sultan, Miri</t>
+          <t>6349 Marissa Pass Suite 370
+Sethton, WY 82983</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -2035,7 +2057,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>S**********r</t>
+          <t>Todd Martinez</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -2048,7 +2070,8 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>467, Jalan King, Kuching</t>
+          <t>PSC 3488, Box 2229
+APO AA 43527</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -2104,7 +2127,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>N********h</t>
+          <t>Rodney Rangel</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -2117,7 +2140,8 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>489, Jalan Tunku, Klang</t>
+          <t>28088 John Mall
+Terrishire, IA 76401</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -2173,7 +2197,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>L*********i</t>
+          <t>Ashley Brown</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -2186,7 +2210,8 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>501, Jalan Taman, Georgetown</t>
+          <t>5591 Baker Groves Suite 620
+Lorimouth, AL 54896</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -2242,7 +2267,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>A********j</t>
+          <t>Dr. Mark Delgado</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -2255,7 +2280,8 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>523, Jalan Sri, Sibu</t>
+          <t>5612 Jeff Roads Suite 082
+Khanville, RI 13665</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -2311,7 +2337,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>S**************r</t>
+          <t>Michael Williams</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -2324,7 +2350,8 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>545, Jalan Hijau, Kuala Lumpur</t>
+          <t>55013 Catherine Meadow Apt. 040
+North Maurice, SD 76429</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -2380,7 +2407,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>W**********i</t>
+          <t>Wendy Malone</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -2393,7 +2420,8 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>567, Jalan Desa, Putrajaya</t>
+          <t>13621 Michael Harbor
+South Bettyshire, NH 58398</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -2449,7 +2477,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>A**************n</t>
+          <t>Brittany Garcia</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -2462,7 +2490,8 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>589, Jalan Teratai, Sandakan</t>
+          <t>9982 Lawrence Manors Apt. 459
+Davidstad, MN 21595</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -2518,7 +2547,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>K*************n</t>
+          <t>Brian Lucas</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -2531,7 +2560,8 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>601, Jalan Melati, Johor Bahru</t>
+          <t>531 Reilly Trail
+Rayville, TN 94845</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">

</xml_diff>

<commit_message>
Enhanced the data masking logic
</commit_message>
<xml_diff>
--- a/backend/uploads/masked/masked_Student_Information.xlsx
+++ b/backend/uploads/masked/masked_Student_Information.xlsx
@@ -513,28 +513,28 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Jennifer Rodriguez</t>
+          <t>Wayne Lopez</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>9************4</t>
+          <t>9**********4</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>1975-09-27</t>
+          <t>12/11/1992</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>92966 Brandon Canyon Suite 730
-Dayland, IN 71365</t>
+          <t>USCGC Willis
+FPO AP 35902</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0*********9</t>
+          <t>***-*****89</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -549,7 +549,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Kuala Lumpur</t>
+          <t>Smithburgh</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -558,7 +558,7 @@
         </is>
       </c>
       <c r="J2" t="n">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
@@ -571,42 +571,42 @@
         </is>
       </c>
       <c r="M2" t="n">
-        <v>5000</v>
+        <v>3582</v>
       </c>
       <c r="N2" t="n">
         <v>3.5</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>Computer Science 1A</t>
+          <t>population</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Susan Chapman</t>
+          <t>Nichole Parsons</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>9************5</t>
+          <t>9**********5</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>1972-02-12</t>
+          <t>30/05/1957</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>92484 Sanchez Burg Suite 331
-Grayland, OK 72314</t>
+          <t>97135 Boyd Glen
+Mcdanielmouth, VA 10567</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0*********0</t>
+          <t>***-*****90</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -621,7 +621,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Johor Bahru</t>
+          <t>West Crystalfurt</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -630,7 +630,7 @@
         </is>
       </c>
       <c r="J3" t="n">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
@@ -643,42 +643,42 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>4500</v>
+        <v>7177</v>
       </c>
       <c r="N3" t="n">
         <v>3.8</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Business Admin 2B</t>
+          <t>cause</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Tina Elliott</t>
+          <t>Linda Bailey</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>9************6</t>
+          <t>9**********6</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1926-05-04</t>
+          <t>10/08/1997</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>9373 Stacy Unions Suite 449
-Cannonland, IA 21742</t>
+          <t>937 Foster Walks
+Grossstad, DE 27171</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0*********1</t>
+          <t>***-*****01</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -693,7 +693,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Penang</t>
+          <t>West Trevor</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="J4" t="n">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
@@ -715,42 +715,42 @@
         </is>
       </c>
       <c r="M4" t="n">
-        <v>6000</v>
+        <v>9711</v>
       </c>
       <c r="N4" t="n">
         <v>3.4</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Engineering 3C</t>
+          <t>enjoy</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Nicholas Wells</t>
+          <t>Joshua Flores</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>9************7</t>
+          <t>9**********7</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1925-11-10</t>
+          <t>17/02/1927</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>677 Ronald Lights
-Andrewchester, AS 30654</t>
+          <t>PSC 4065, Box 0678
+APO AE 60035</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0*********2</t>
+          <t>***-*****12</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -765,7 +765,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Ipoh</t>
+          <t>West Bethbury</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -774,7 +774,7 @@
         </is>
       </c>
       <c r="J5" t="n">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
@@ -787,42 +787,42 @@
         </is>
       </c>
       <c r="M5" t="n">
-        <v>5500</v>
+        <v>4186</v>
       </c>
       <c r="N5" t="n">
         <v>3.6</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>Medicine 4D</t>
+          <t>record</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Shawn Hunt</t>
+          <t>Robert Salas</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>9************8</t>
+          <t>9**********8</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1976-07-02</t>
+          <t>28/10/1996</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>471 Bryan Fields
-Georgestad, NJ 77162</t>
+          <t>2001 Nicole Avenue
+Patrickfurt, PW 94092</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0*********3</t>
+          <t>***-*****23</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -837,7 +837,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Shah Alam</t>
+          <t>Lake Kennethstad</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -846,7 +846,7 @@
         </is>
       </c>
       <c r="J6" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
@@ -859,42 +859,42 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>5200</v>
+        <v>6285</v>
       </c>
       <c r="N6" t="n">
         <v>3.7</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>Law 5E</t>
+          <t>growth</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Kristen Fox</t>
+          <t>Jason Johnson</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>9************9</t>
+          <t>9**********9</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1957-01-29</t>
+          <t>24/12/1992</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>075 Macias Curve Suite 296
-Lopezborough, NH 38025</t>
+          <t>696 Thomas Views Suite 830
+East Marymouth, WI 73270</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0*********4</t>
+          <t>***-*****34</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -909,7 +909,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Melaka</t>
+          <t>Jacksonmouth</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -918,7 +918,7 @@
         </is>
       </c>
       <c r="J7" t="n">
-        <v>27</v>
+        <v>90</v>
       </c>
       <c r="K7" t="inlineStr">
         <is>
@@ -931,42 +931,42 @@
         </is>
       </c>
       <c r="M7" t="n">
-        <v>4800</v>
+        <v>6755</v>
       </c>
       <c r="N7" t="n">
         <v>3.9</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Nursing 6F</t>
+          <t>wear</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Madison Duncan</t>
+          <t>Alejandro Francis</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>9************0</t>
+          <t>9**********0</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1947-02-06</t>
+          <t>04/09/1962</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>75232 Walters Pines
-Jasonborough, OK 27600</t>
+          <t>754 Perez Prairie
+North Rogerfort, KY 48698</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>0*********5</t>
+          <t>***-*****45</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -981,7 +981,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Seremban</t>
+          <t>Powerstown</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -990,7 +990,7 @@
         </is>
       </c>
       <c r="J8" t="n">
-        <v>26</v>
+        <v>76</v>
       </c>
       <c r="K8" t="inlineStr">
         <is>
@@ -1003,42 +1003,42 @@
         </is>
       </c>
       <c r="M8" t="n">
-        <v>5300</v>
+        <v>7073</v>
       </c>
       <c r="N8" t="n">
         <v>3.45</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Architecture 7G</t>
+          <t>analysis</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Laurie Holmes</t>
+          <t>Stephanie Roberts</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>9************1</t>
+          <t>9**********1</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1928-07-24</t>
+          <t>19/08/1930</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>595 Brenda Harbor Suite 060
-South Madisonfurt, AZ 49540</t>
+          <t>494 Hess Place
+Fosterburgh, RI 34180</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>0*********6</t>
+          <t>***-*****56</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1053,7 +1053,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Kuantan</t>
+          <t>Aprilburgh</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -1062,7 +1062,7 @@
         </is>
       </c>
       <c r="J9" t="n">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="K9" t="inlineStr">
         <is>
@@ -1075,42 +1075,42 @@
         </is>
       </c>
       <c r="M9" t="n">
-        <v>4700</v>
+        <v>2351</v>
       </c>
       <c r="N9" t="n">
         <v>3.65</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Pharmacy 8H</t>
+          <t>information</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Christina Espinoza</t>
+          <t>Karen Burton</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>0************2</t>
+          <t>0**********2</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1975-03-10</t>
+          <t>10/12/1934</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>PSC 8157, Box 1769
-APO AA 76606</t>
+          <t>69310 Jessica Rest
+Michaelstad, SC 81770</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>0*********8</t>
+          <t>***-*****78</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1125,7 +1125,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Kota Kinabalu</t>
+          <t>Lake Roberthaven</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -1134,7 +1134,7 @@
         </is>
       </c>
       <c r="J10" t="n">
-        <v>24</v>
+        <v>89</v>
       </c>
       <c r="K10" t="inlineStr">
         <is>
@@ -1147,42 +1147,42 @@
         </is>
       </c>
       <c r="M10" t="n">
-        <v>6200</v>
+        <v>9135</v>
       </c>
       <c r="N10" t="n">
         <v>3.75</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Accounting 9I</t>
+          <t>hit</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Brenda Petersen</t>
+          <t>Justin Rodriguez</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>0************3</t>
+          <t>0**********3</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2004-02-25</t>
+          <t>24/06/1934</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>566 Kevin Cliffs
-Port Carlos, AL 04739</t>
+          <t>Unit 0240 Box 1862
+DPO AP 15594</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>0*********9</t>
+          <t>***-*****89</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1197,7 +1197,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Kuala Terengganu</t>
+          <t>Georgeton</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -1206,7 +1206,7 @@
         </is>
       </c>
       <c r="J11" t="n">
-        <v>23</v>
+        <v>74</v>
       </c>
       <c r="K11" t="inlineStr">
         <is>
@@ -1219,42 +1219,42 @@
         </is>
       </c>
       <c r="M11" t="n">
-        <v>4900</v>
+        <v>9272</v>
       </c>
       <c r="N11" t="n">
         <v>3.85</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Biotechnology 10J</t>
+          <t>man</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Sharon Owen</t>
+          <t>Maureen Rivera</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>0************4</t>
+          <t>0**********4</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1939-12-02</t>
+          <t>10/04/1957</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>247 Felicia Keys
-Port Mary, NY 16973</t>
+          <t>9839 Mcmillan Lights Apt. 704
+Johnmouth, RI 68936</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>0*********1</t>
+          <t>***-*****01</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1269,7 +1269,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Alor Setar</t>
+          <t>East Peter</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -1278,7 +1278,7 @@
         </is>
       </c>
       <c r="J12" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="K12" t="inlineStr">
         <is>
@@ -1291,42 +1291,42 @@
         </is>
       </c>
       <c r="M12" t="n">
-        <v>4500</v>
+        <v>4605</v>
       </c>
       <c r="N12" t="n">
         <v>3.55</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Psychology 11K</t>
+          <t>election</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Ashley Gonzales</t>
+          <t>Darryl Weiss</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>0************5</t>
+          <t>0**********5</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>1979-02-24</t>
+          <t>04/09/1930</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>158 David Trafficway
-Katherinechester, AS 45943</t>
+          <t>Unit 5002 Box 8334
+DPO AA 76006</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>0*********2</t>
+          <t>***-*****12</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1341,7 +1341,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Miri</t>
+          <t>West Molly</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -1350,7 +1350,7 @@
         </is>
       </c>
       <c r="J13" t="n">
-        <v>21</v>
+        <v>95</v>
       </c>
       <c r="K13" t="inlineStr">
         <is>
@@ -1363,42 +1363,42 @@
         </is>
       </c>
       <c r="M13" t="n">
-        <v>5800</v>
+        <v>8922</v>
       </c>
       <c r="N13" t="n">
         <v>3.5</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Chemistry 12L</t>
+          <t>help</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>David Myers</t>
+          <t>Daniel Walker</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>0************6</t>
+          <t>0**********6</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>1993-02-25</t>
+          <t>10/12/1929</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>4817 Tonya Meadows
-Johnstad, OK 61309</t>
+          <t>935 Morgan Drives
+Ryanport, OR 60678</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>0*********3</t>
+          <t>***-*****23</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1413,7 +1413,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Kuching</t>
+          <t>Anthonytown</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1422,7 +1422,7 @@
         </is>
       </c>
       <c r="J14" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="K14" t="inlineStr">
         <is>
@@ -1435,42 +1435,42 @@
         </is>
       </c>
       <c r="M14" t="n">
-        <v>5600</v>
+        <v>7886</v>
       </c>
       <c r="N14" t="n">
         <v>3.6</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Physics 13M</t>
+          <t>difference</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Ricky Sherman</t>
+          <t>Stephen Clark</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>0************7</t>
+          <t>0**********7</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>1957-04-19</t>
+          <t>25/08/1985</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>71763 Harris Point
-East Casey, RI 14476</t>
+          <t>21848 Avila Court
+West Brandon, WA 47870</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>0*********4</t>
+          <t>***-*****34</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1485,7 +1485,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Klang</t>
+          <t>Caitlinmouth</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1494,7 +1494,7 @@
         </is>
       </c>
       <c r="J15" t="n">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="K15" t="inlineStr">
         <is>
@@ -1507,42 +1507,42 @@
         </is>
       </c>
       <c r="M15" t="n">
-        <v>4700</v>
+        <v>7500</v>
       </c>
       <c r="N15" t="n">
         <v>3.8</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Mathematics 14N</t>
+          <t>pattern</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Nicholas Petersen</t>
+          <t>Travis Mccall</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>0************8</t>
+          <t>0**********8</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1984-05-13</t>
+          <t>14/04/1951</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>381 Destiny Track
-Edwinview, ID 24102</t>
+          <t>3511 Thomas Way
+Port Jamesstad, NM 25197</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>0*********5</t>
+          <t>***-*****45</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1557,7 +1557,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Georgetown</t>
+          <t>East Samuel</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -1566,7 +1566,7 @@
         </is>
       </c>
       <c r="J16" t="n">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="K16" t="inlineStr">
         <is>
@@ -1579,42 +1579,42 @@
         </is>
       </c>
       <c r="M16" t="n">
-        <v>4900</v>
+        <v>9736</v>
       </c>
       <c r="N16" t="n">
         <v>3.7</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>Economics 15O</t>
+          <t>I</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Daniel Garcia</t>
+          <t>Joshua Garcia</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>0************9</t>
+          <t>0**********9</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1943-05-17</t>
+          <t>16/07/2006</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>PSC 3371, Box 6888
-APO AE 68523</t>
+          <t>3293 Gary Drive Suite 787
+South Krista, NM 37393</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>0*********6</t>
+          <t>***-*****56</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1629,7 +1629,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Kuala Lumpur</t>
+          <t>West Mariehaven</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -1638,7 +1638,7 @@
         </is>
       </c>
       <c r="J17" t="n">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="K17" t="inlineStr">
         <is>
@@ -1651,42 +1651,42 @@
         </is>
       </c>
       <c r="M17" t="n">
-        <v>4600</v>
+        <v>4714</v>
       </c>
       <c r="N17" t="n">
         <v>3.75</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>History 16P</t>
+          <t>collection</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Vicki Morgan</t>
+          <t>Christopher Carrillo</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>0************0</t>
+          <t>0**********0</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1983-09-16</t>
+          <t>13/02/1983</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>091 Fischer Dale
-Andreamouth, CT 33331</t>
+          <t>8515 Thomas Parks
+Clineborough, NV 61599</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>0*********7</t>
+          <t>***-*****67</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1701,7 +1701,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Putrajaya</t>
+          <t>Port Cindy</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -1710,7 +1710,7 @@
         </is>
       </c>
       <c r="J18" t="n">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="K18" t="inlineStr">
         <is>
@@ -1723,42 +1723,42 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>5100</v>
+        <v>2942</v>
       </c>
       <c r="N18" t="n">
         <v>3.65</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Political Sci 17Q</t>
+          <t>outside</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Nicholas Davila</t>
+          <t>Lindsey Klein</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>0************1</t>
+          <t>0**********1</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1939-09-09</t>
+          <t>09/05/1980</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>235 White Hills Apt. 307
-Andrewsville, GA 56368</t>
+          <t>890 John Corners Apt. 904
+Lake Lisaland, NY 94693</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>0*********8</t>
+          <t>***-*****78</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1773,7 +1773,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Sibu</t>
+          <t>Danielland</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -1782,7 +1782,7 @@
         </is>
       </c>
       <c r="J19" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="K19" t="inlineStr">
         <is>
@@ -1795,42 +1795,42 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>5200</v>
+        <v>8815</v>
       </c>
       <c r="N19" t="n">
         <v>3.85</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Sociology 18R</t>
+          <t>example</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Alyssa Campos</t>
+          <t>Ariel Rubio</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>1************2</t>
+          <t>1**********2</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1998-02-06</t>
+          <t>18/07/1980</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>384 Matthew Island
-Torresland, MO 57458</t>
+          <t>8090 Jason Rue Suite 045
+Lake Stevenmouth, AS 90385</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>0*********9</t>
+          <t>***-*****89</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1845,7 +1845,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Sandakan</t>
+          <t>South Kimberlyfurt</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -1854,7 +1854,7 @@
         </is>
       </c>
       <c r="J20" t="n">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="K20" t="inlineStr">
         <is>
@@ -1867,42 +1867,42 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>4700</v>
+        <v>9754</v>
       </c>
       <c r="N20" t="n">
         <v>3.5</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Computer Science 19S</t>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>James Jones</t>
+          <t>Alexis Hoover DVM</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>1************3</t>
+          <t>1**********3</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1976-05-01</t>
+          <t>07/03/1993</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Unit 4917 Box 9699
-DPO AA 69452</t>
+          <t>20036 Lori Islands Suite 642
+Lake Christopher, MO 43411</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>0*********0</t>
+          <t>***-*****90</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1917,7 +1917,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Kuala Lumpur</t>
+          <t>West Steventown</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -1926,7 +1926,7 @@
         </is>
       </c>
       <c r="J21" t="n">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="K21" t="inlineStr">
         <is>
@@ -1939,42 +1939,42 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>4300</v>
+        <v>6085</v>
       </c>
       <c r="N21" t="n">
         <v>3.55</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Business Admin 20T</t>
+          <t>manager</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Jamie Adkins</t>
+          <t>Jermaine Sims</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>1************4</t>
+          <t>1**********4</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1960-07-12</t>
+          <t>05/09/1941</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>0269 Timothy Island Suite 786
-North Joshua, NJ 16285</t>
+          <t>138 Roberts Ports
+Port Suzanne, PA 03681</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>0*********1</t>
+          <t>***-*****01</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1989,7 +1989,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Alor Setar</t>
+          <t>East Jay</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -1998,7 +1998,7 @@
         </is>
       </c>
       <c r="J22" t="n">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="K22" t="inlineStr">
         <is>
@@ -2011,42 +2011,42 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>4600</v>
+        <v>2072</v>
       </c>
       <c r="N22" t="n">
         <v>3.8</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Education 21U</t>
+          <t>head</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Alyssa Torres</t>
+          <t>Laurie Bell DVM</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>1************5</t>
+          <t>1**********5</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>1995-12-22</t>
+          <t>23/03/1941</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>29927 Timothy Trafficway Apt. 293
-North Carla, HI 04674</t>
+          <t>Unit 2160 Box 6707
+DPO AE 26701</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>0*********2</t>
+          <t>***-*****12</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2061,7 +2061,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Miri</t>
+          <t>Stephaniestad</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -2070,7 +2070,7 @@
         </is>
       </c>
       <c r="J23" t="n">
-        <v>11</v>
+        <v>79</v>
       </c>
       <c r="K23" t="inlineStr">
         <is>
@@ -2083,42 +2083,42 @@
         </is>
       </c>
       <c r="M23" t="n">
-        <v>5500</v>
+        <v>8977</v>
       </c>
       <c r="N23" t="n">
         <v>3.65</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Literature 22V</t>
+          <t>last</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Dr. Ashley Padilla</t>
+          <t>Robert Duncan</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>1************6</t>
+          <t>1**********6</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>1934-10-22</t>
+          <t>28/04/1995</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>90193 Diana Creek
-Leestad, DE 39643</t>
+          <t>4296 King Creek Apt. 808
+North Ellen, AK 29042</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>0*********3</t>
+          <t>***-*****23</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2133,7 +2133,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Kuching</t>
+          <t>Port Lacey</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
@@ -2142,7 +2142,7 @@
         </is>
       </c>
       <c r="J24" t="n">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="K24" t="inlineStr">
         <is>
@@ -2155,42 +2155,42 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>4800</v>
+        <v>8937</v>
       </c>
       <c r="N24" t="n">
         <v>3.75</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Geography 23W</t>
+          <t>lay</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>David Burch</t>
+          <t>Dawn Pham</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>1************7</t>
+          <t>1**********7</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>1979-05-16</t>
+          <t>13/09/1971</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>44613 Jamie Orchard Apt. 408
-Sparksstad, KY 54863</t>
+          <t>1533 Laurie Corners Apt. 680
+South Christopher, MD 13700</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>0*********4</t>
+          <t>***-*****34</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2205,7 +2205,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Klang</t>
+          <t>East Ronaldland</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -2214,7 +2214,7 @@
         </is>
       </c>
       <c r="J25" t="n">
-        <v>9</v>
+        <v>91</v>
       </c>
       <c r="K25" t="inlineStr">
         <is>
@@ -2227,42 +2227,42 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>4500</v>
+        <v>7945</v>
       </c>
       <c r="N25" t="n">
         <v>3.85</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Art 24X</t>
+          <t>modern</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Tiffany Riley</t>
+          <t>Kathy Powell</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>1************8</t>
+          <t>1**********8</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>1995-09-17</t>
+          <t>11/03/1931</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>570 Rogers Locks Apt. 277
-East Juliastad, PR 81704</t>
+          <t>586 Long Trail
+Port Laurieland, MA 84267</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>0*********5</t>
+          <t>***-*****45</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2277,7 +2277,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Georgetown</t>
+          <t>Lake Brian</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -2286,7 +2286,7 @@
         </is>
       </c>
       <c r="J26" t="n">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="K26" t="inlineStr">
         <is>
@@ -2299,42 +2299,42 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>5200</v>
+        <v>3367</v>
       </c>
       <c r="N26" t="n">
         <v>3.9</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Music 25Y</t>
+          <t>world</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Curtis Joyce MD</t>
+          <t>Kimberly Gray</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>1************9</t>
+          <t>1**********9</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>1974-07-23</t>
+          <t>09/03/1962</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>PSC 3796, Box 8239
-APO AA 82046</t>
+          <t>168 Philip Knolls
+Kathrynside, ID 60944</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>0*********6</t>
+          <t>***-*****56</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2349,7 +2349,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Sibu</t>
+          <t>Espinozaside</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -2358,7 +2358,7 @@
         </is>
       </c>
       <c r="J27" t="n">
-        <v>7</v>
+        <v>95</v>
       </c>
       <c r="K27" t="inlineStr">
         <is>
@@ -2371,42 +2371,42 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>5400</v>
+        <v>5531</v>
       </c>
       <c r="N27" t="n">
         <v>3.8</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Dance 26Z</t>
+          <t>marriage</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Jessica Miller</t>
+          <t>Kathryn White</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>1************0</t>
+          <t>1**********0</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>1933-09-27</t>
+          <t>21/01/1939</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>4125 Bell Trail
-Ryanfurt, AL 44201</t>
+          <t>729 Derek Highway Suite 964
+Jeffreyhaven, CO 81240</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>0*********7</t>
+          <t>***-*****67</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2421,7 +2421,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Kuala Lumpur</t>
+          <t>Lake Bryan</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -2430,7 +2430,7 @@
         </is>
       </c>
       <c r="J28" t="n">
-        <v>6</v>
+        <v>49</v>
       </c>
       <c r="K28" t="inlineStr">
         <is>
@@ -2443,42 +2443,42 @@
         </is>
       </c>
       <c r="M28" t="n">
-        <v>5000</v>
+        <v>6700</v>
       </c>
       <c r="N28" t="n">
         <v>3.65</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Theatre 27A</t>
+          <t>decide</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Alexa Ross</t>
+          <t>Nicole Kidd</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>1************1</t>
+          <t>1**********1</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>1946-07-30</t>
+          <t>20/10/1974</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>18124 Gary Cove Suite 762
-New Jessicaport, CA 14465</t>
+          <t>0339 Cameron Brooks Apt. 639
+East Chad, AS 35485</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>0*********8</t>
+          <t>***-*****78</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2493,7 +2493,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Putrajaya</t>
+          <t>North Davidfurt</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -2502,7 +2502,7 @@
         </is>
       </c>
       <c r="J29" t="n">
-        <v>5</v>
+        <v>77</v>
       </c>
       <c r="K29" t="inlineStr">
         <is>
@@ -2515,42 +2515,42 @@
         </is>
       </c>
       <c r="M29" t="n">
-        <v>5800</v>
+        <v>4686</v>
       </c>
       <c r="N29" t="n">
         <v>3.7</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Culinary Arts 28B</t>
+          <t>voice</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Mary Kelly</t>
+          <t>Justin Oneal</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>2************2</t>
+          <t>2**********2</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1930-06-05</t>
+          <t>25/10/1959</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>USS Beard
-FPO AP 77606</t>
+          <t>892 Allen Terrace Suite 908
+Annaville, KY 05160</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>0*********9</t>
+          <t>***-*****89</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2565,7 +2565,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Sandakan</t>
+          <t>Lake Jessebury</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -2574,7 +2574,7 @@
         </is>
       </c>
       <c r="J30" t="n">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="K30" t="inlineStr">
         <is>
@@ -2587,42 +2587,42 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>4700</v>
+        <v>7574</v>
       </c>
       <c r="N30" t="n">
         <v>3.85</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Fashion Design 29C</t>
+          <t>fish</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Mary Lopez</t>
+          <t>Janice Ibarra</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>2************3</t>
+          <t>2**********3</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>2001-03-16</t>
+          <t>28/01/2000</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>377 Melissa Cliff
-New Kevin, NM 46953</t>
+          <t>PSC 1569, Box 9608
+APO AP 45134</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>0*********0</t>
+          <t>***-*****90</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2637,7 +2637,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Johor Bahru</t>
+          <t>Leemouth</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
@@ -2646,7 +2646,7 @@
         </is>
       </c>
       <c r="J31" t="n">
-        <v>3</v>
+        <v>74</v>
       </c>
       <c r="K31" t="inlineStr">
         <is>
@@ -2659,14 +2659,14 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>4900</v>
+        <v>9315</v>
       </c>
       <c r="N31" t="n">
         <v>3.55</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Photography 30D</t>
+          <t>hospital</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Enhanced the masking logic
</commit_message>
<xml_diff>
--- a/backend/uploads/masked/masked_Student_Information.xlsx
+++ b/backend/uploads/masked/masked_Student_Information.xlsx
@@ -513,7 +513,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Joseph Calderon</t>
+          <t>Lisa Adams</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -523,13 +523,13 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>24/08/1988</t>
+          <t>19/02/1995</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>29238 Benjamin Knoll Suite 887
-West Ashleyhaven, AS 57961</t>
+          <t>29005 Bryan Heights
+Port Sarahhaven, DE 77487</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -539,7 +539,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Pressure recently.</t>
+          <t>The meeting myself.</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -549,43 +549,43 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Josephmouth</t>
+          <t>South Shannon</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Single ten long.</t>
+          <t>Size one health he.</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>29</v>
+        <v>77</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Figure huge care.</t>
+          <t>Partner too risk.</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Defense decade view.</t>
+          <t>Truth view score.</t>
         </is>
       </c>
       <c r="M2" t="n">
-        <v>5534</v>
+        <v>2053</v>
       </c>
       <c r="N2" t="n">
-        <v>7227</v>
+        <v>6377</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>interesting</t>
+          <t>standard</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Wesley White</t>
+          <t>Sandra Rogers</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -595,13 +595,13 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>10/01/1962</t>
+          <t>29/01/1999</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>66919 Gonzalez Coves
-South Brooke, AR 73683</t>
+          <t>9244 Franklin Oval Apt. 569
+Michealborough, IL 45211</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -611,7 +611,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Agent picture.</t>
+          <t>Alone tell support.</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -621,43 +621,43 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Georgehaven</t>
+          <t>Lake Lori</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Design natural.</t>
+          <t>Wrong newspaper per.</t>
         </is>
       </c>
       <c r="J3" t="n">
-        <v>96</v>
+        <v>35</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Economic fall free.</t>
+          <t>Democrat fly people.</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Their society argue.</t>
+          <t>Difficult data.</t>
         </is>
       </c>
       <c r="M3" t="n">
-        <v>2244</v>
+        <v>4599</v>
       </c>
       <c r="N3" t="n">
-        <v>3325</v>
+        <v>2124</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>scene</t>
+          <t>vote</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Nicole Calhoun</t>
+          <t>Jason Hogan</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -667,13 +667,13 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>25/04/1988</t>
+          <t>05/03/2005</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>67520 Hines Pike
-Benjaminport, MH 25043</t>
+          <t>Unit 8170 Box 4535
+DPO AP 31029</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -683,7 +683,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Hundred single view.</t>
+          <t>Consider reflect.</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -693,43 +693,43 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Brownchester</t>
+          <t>New Brookefort</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Report put card man.</t>
+          <t>Parent contain ago.</t>
         </is>
       </c>
       <c r="J4" t="n">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Fear admit get.</t>
+          <t>Leave son market.</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Similar prevent.</t>
+          <t>Pay which mention.</t>
         </is>
       </c>
       <c r="M4" t="n">
-        <v>3181</v>
+        <v>8454</v>
       </c>
       <c r="N4" t="n">
-        <v>5934</v>
+        <v>1011</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>else</t>
+          <t>something</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Cynthia Hawkins</t>
+          <t>Diana Owens</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -739,13 +739,13 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>06/03/1994</t>
+          <t>23/12/1958</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>PSC 0059, Box 7134
-APO AP 66319</t>
+          <t>711 Kellie Road
+South Jason, OH 41719</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -755,7 +755,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Guy thought officer.</t>
+          <t>Carry citizen chair.</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -765,43 +765,43 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Richardstad</t>
+          <t>New Sherryshire</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Security hotel lot.</t>
+          <t>Hotel cup project.</t>
         </is>
       </c>
       <c r="J5" t="n">
-        <v>62</v>
+        <v>34</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Experience region.</t>
+          <t>Somebody own.</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>Receive surface.</t>
+          <t>Light these teach.</t>
         </is>
       </c>
       <c r="M5" t="n">
-        <v>6866</v>
+        <v>2195</v>
       </c>
       <c r="N5" t="n">
-        <v>2066</v>
+        <v>1197</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>return</t>
+          <t>lot</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Douglas Wagner</t>
+          <t>Stuart Santiago</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -811,13 +811,13 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>11/07/1979</t>
+          <t>19/10/1957</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>313 Campbell Ridge Apt. 301
-Douglasburgh, PR 79132</t>
+          <t>USS Guzman
+FPO AA 39720</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -827,7 +827,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Mr something.</t>
+          <t>Agency call but.</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -837,43 +837,43 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Maxwellport</t>
+          <t>Adriantown</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Decade raise center.</t>
+          <t>Head through.</t>
         </is>
       </c>
       <c r="J6" t="n">
-        <v>58</v>
+        <v>100</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Television street.</t>
+          <t>Wall sport free air.</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>Carry old rule I.</t>
+          <t>Race myself fish.</t>
         </is>
       </c>
       <c r="M6" t="n">
-        <v>4288</v>
+        <v>2921</v>
       </c>
       <c r="N6" t="n">
-        <v>7790</v>
+        <v>9787</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>style</t>
+          <t>about</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Caitlin Spears</t>
+          <t>Jeffrey Holloway</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -883,13 +883,13 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>01/10/1999</t>
+          <t>24/02/1942</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>USNV Hall
-FPO AE 67787</t>
+          <t>439 Wendy Via
+Lisahaven, UT 17632</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -899,7 +899,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Box affect activity.</t>
+          <t>Wonder fast.</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -909,43 +909,43 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>North Karenview</t>
+          <t>New Julia</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Wide question ahead.</t>
+          <t>Again use key store.</t>
         </is>
       </c>
       <c r="J7" t="n">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Series new.</t>
+          <t>Be position.</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Win explain black.</t>
+          <t>Make style figure.</t>
         </is>
       </c>
       <c r="M7" t="n">
-        <v>6039</v>
+        <v>7749</v>
       </c>
       <c r="N7" t="n">
-        <v>4678</v>
+        <v>8018</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>similar</t>
+          <t>administration</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Robert Gould</t>
+          <t>Nicholas Mitchell</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -955,13 +955,13 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>11/08/1994</t>
+          <t>02/02/1993</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>054 Christopher Springs Apt. 722
-Lake Sheilatown, VA 86006</t>
+          <t>204 Cole Plains
+Port Justin, MS 95954</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -971,7 +971,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Green specific fish.</t>
+          <t>Skin white.</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -981,43 +981,43 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>New Kathrynview</t>
+          <t>Port Nicoleland</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Concern majority.</t>
+          <t>National side no.</t>
         </is>
       </c>
       <c r="J8" t="n">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Security test major.</t>
+          <t>Agent box specific.</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>Born which art team.</t>
+          <t>Interview floor.</t>
         </is>
       </c>
       <c r="M8" t="n">
-        <v>6920</v>
+        <v>7890</v>
       </c>
       <c r="N8" t="n">
-        <v>4381</v>
+        <v>8225</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>thousand</t>
+          <t>individual</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Roger Mueller</t>
+          <t>Ricardo Davis</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1027,13 +1027,13 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>07/11/2001</t>
+          <t>15/02/1986</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>69045 Bennett Dale
-Lake Christopher, UT 52529</t>
+          <t>09863 Jessica Estates
+North Marc, VA 19730</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -1043,7 +1043,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Bill station play.</t>
+          <t>Still partner next.</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -1053,43 +1053,43 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Carsonshire</t>
+          <t>Charlesstad</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>TV state type focus.</t>
+          <t>Practice husband.</t>
         </is>
       </c>
       <c r="J9" t="n">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Available save main.</t>
+          <t>Together collection.</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>Energy represent.</t>
+          <t>Pretty cover.</t>
         </is>
       </c>
       <c r="M9" t="n">
-        <v>9810</v>
+        <v>9308</v>
       </c>
       <c r="N9" t="n">
-        <v>3805</v>
+        <v>7326</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>herself</t>
+          <t>edge</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>George Mckenzie</t>
+          <t>Brett Scott</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1099,13 +1099,13 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>18/05/1961</t>
+          <t>19/09/1967</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>31685 Amanda Stravenue
-New Carly, VT 67763</t>
+          <t>Unit 8558 Box 3894
+DPO AP 85220</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -1115,7 +1115,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Positive probably.</t>
+          <t>State because.</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -1125,43 +1125,43 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Cowanfort</t>
+          <t>South Sarah</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Magazine tax send.</t>
+          <t>Write sense note.</t>
         </is>
       </c>
       <c r="J10" t="n">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Provide born which.</t>
+          <t>Special bring hour.</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>List team.</t>
+          <t>Behind order stand.</t>
         </is>
       </c>
       <c r="M10" t="n">
-        <v>8154</v>
+        <v>6035</v>
       </c>
       <c r="N10" t="n">
-        <v>5500</v>
+        <v>4074</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>spend</t>
+          <t>race</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Brian Tucker</t>
+          <t>Richard Howard</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1171,13 +1171,13 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>24/03/1988</t>
+          <t>18/09/1993</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>57715 Patricia Landing
-West Pamelaborough, MA 07937</t>
+          <t>073 Robinson Unions Suite 180
+Hebertview, AS 83530</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -1187,7 +1187,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Still Mrs radio.</t>
+          <t>Both hospital send.</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -1197,43 +1197,43 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Cookton</t>
+          <t>East Craig</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Technology grow.</t>
+          <t>Attorney front.</t>
         </is>
       </c>
       <c r="J11" t="n">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>Behavior recognize.</t>
+          <t>Series chance may.</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>Expect couple pass.</t>
+          <t>Challenge structure.</t>
         </is>
       </c>
       <c r="M11" t="n">
-        <v>7638</v>
+        <v>2042</v>
       </c>
       <c r="N11" t="n">
-        <v>5161</v>
+        <v>6804</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>goal</t>
+          <t>create</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Richard Williams</t>
+          <t>Drew Kane</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1243,13 +1243,13 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>21/05/2005</t>
+          <t>18/07/1946</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>USNV Tanner
-FPO AE 32082</t>
+          <t>PSC 5825, Box 1127
+APO AE 53983</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -1259,7 +1259,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Trip environment.</t>
+          <t>Street worry just.</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -1269,43 +1269,43 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Kendraton</t>
+          <t>Port Michaelborough</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>Moment husband.</t>
+          <t>How group stuff.</t>
         </is>
       </c>
       <c r="J12" t="n">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>Really history.</t>
+          <t>Look heavy wonder.</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>Sometimes edge.</t>
+          <t>Tough force early.</t>
         </is>
       </c>
       <c r="M12" t="n">
-        <v>3870</v>
+        <v>4678</v>
       </c>
       <c r="N12" t="n">
-        <v>7596</v>
+        <v>2204</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>hit</t>
+          <t>phone</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Carol Garrison</t>
+          <t>Yvonne Taylor</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1315,13 +1315,13 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>09/04/1982</t>
+          <t>26/03/1942</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>6663 Tamara Ridges
-East Micheal, NM 53220</t>
+          <t>6254 Susan Plaza Apt. 256
+South Daniel, CT 46017</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -1331,7 +1331,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Trade recognize.</t>
+          <t>Outside sing save.</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -1341,43 +1341,43 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Calvinbury</t>
+          <t>East Lacey</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>Population feeling.</t>
+          <t>Light dark letter.</t>
         </is>
       </c>
       <c r="J13" t="n">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Apply discussion.</t>
+          <t>Conference player.</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>Again section later.</t>
+          <t>The remember them.</t>
         </is>
       </c>
       <c r="M13" t="n">
-        <v>7658</v>
+        <v>2673</v>
       </c>
       <c r="N13" t="n">
-        <v>4441</v>
+        <v>5481</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>yourself</t>
+          <t>style</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Mitchell Sparks</t>
+          <t>Jose Rivera</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1387,13 +1387,13 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>15/08/1951</t>
+          <t>27/02/1967</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>24186 Sarah Lights Apt. 032
-West Darryl, MS 74171</t>
+          <t>28283 Williams Ford Apt. 175
+East Caleb, WA 75733</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1403,7 +1403,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Air fish body area.</t>
+          <t>Cell describe.</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -1413,43 +1413,43 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Randalltown</t>
+          <t>Francohaven</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>Wrong glass hope.</t>
+          <t>Left mission lose.</t>
         </is>
       </c>
       <c r="J14" t="n">
-        <v>54</v>
+        <v>86</v>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>Tell health base.</t>
+          <t>Item physical film.</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Cell image.</t>
+          <t>Charge above.</t>
         </is>
       </c>
       <c r="M14" t="n">
-        <v>8753</v>
+        <v>4381</v>
       </c>
       <c r="N14" t="n">
-        <v>3131</v>
+        <v>8882</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>day</t>
+          <t>project</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Karen Morrison MD</t>
+          <t>Kelly Harrison</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1459,13 +1459,13 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>16/12/1967</t>
+          <t>18/10/2002</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>197 Davis Parkways
-Jordanchester, NV 05949</t>
+          <t>357 Deborah Lights
+Butlerfurt, MD 35339</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1475,7 +1475,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Another PM born.</t>
+          <t>Arrive rule within.</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -1485,43 +1485,43 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Butlerfurt</t>
+          <t>South Kevin</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>Read wait pick.</t>
+          <t>Focus thing ok.</t>
         </is>
       </c>
       <c r="J15" t="n">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>Employee card.</t>
+          <t>It agreement stock.</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>Thought within.</t>
+          <t>Dog might daughter.</t>
         </is>
       </c>
       <c r="M15" t="n">
-        <v>3804</v>
+        <v>6505</v>
       </c>
       <c r="N15" t="n">
-        <v>6534</v>
+        <v>3092</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>put</t>
+          <t>measure</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Susan Watson</t>
+          <t>Frank Walker</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1531,13 +1531,13 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>17/02/1949</t>
+          <t>23/01/1967</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>19621 Amy Springs
-West Amandatown, SD 62578</t>
+          <t>032 Ruiz Landing
+East Zoechester, MN 26575</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1547,7 +1547,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Appear focus edge.</t>
+          <t>Yes nice us skin.</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1557,43 +1557,43 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Williamfort</t>
+          <t>North Mike</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>His strong total.</t>
+          <t>Cover despite size.</t>
         </is>
       </c>
       <c r="J16" t="n">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>Significant hard.</t>
+          <t>Us forward style.</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>Movement bit their.</t>
+          <t>Word feel seem.</t>
         </is>
       </c>
       <c r="M16" t="n">
-        <v>4485</v>
+        <v>5854</v>
       </c>
       <c r="N16" t="n">
-        <v>8516</v>
+        <v>4999</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>majority</t>
+          <t>easy</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Johnny Howell</t>
+          <t>Dr. Gregory Bell</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1603,13 +1603,13 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>09/06/1934</t>
+          <t>29/07/1974</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>5653 William Vista
-Lake Johntown, MA 43529</t>
+          <t>5091 James Roads Apt. 198
+Ashleyshire, IA 58448</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1619,7 +1619,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Win say hair modern.</t>
+          <t>Trip spend page.</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1629,43 +1629,43 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Figueroaside</t>
+          <t>Hensleyberg</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>Threat note.</t>
+          <t>Environmental pull.</t>
         </is>
       </c>
       <c r="J17" t="n">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>Treat shoulder.</t>
+          <t>Help education.</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>Heart which public.</t>
+          <t>Serve store tonight.</t>
         </is>
       </c>
       <c r="M17" t="n">
-        <v>5930</v>
+        <v>5138</v>
       </c>
       <c r="N17" t="n">
-        <v>4706</v>
+        <v>8357</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>skill</t>
+          <t>cut</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Mr. James Watson</t>
+          <t>James Rangel</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1675,13 +1675,13 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>31/10/1974</t>
+          <t>23/09/1969</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>11550 Barbara Groves Suite 586
-Sanchezfurt, IN 21135</t>
+          <t>5316 Kimberly Lakes
+Brittanyville, AZ 35336</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1691,7 +1691,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Former recently.</t>
+          <t>Wonder technology.</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -1701,12 +1701,12 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Danielleburgh</t>
+          <t>West Timothyside</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>Central over family.</t>
+          <t>Writer join indeed.</t>
         </is>
       </c>
       <c r="J18" t="n">
@@ -1714,30 +1714,30 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Air shake able him.</t>
+          <t>Serve life until.</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>Must no yourself.</t>
+          <t>Mrs card remain.</t>
         </is>
       </c>
       <c r="M18" t="n">
-        <v>7958</v>
+        <v>5712</v>
       </c>
       <c r="N18" t="n">
-        <v>1678</v>
+        <v>2088</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>near</t>
+          <t>figure</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Christina Smith</t>
+          <t>Eric Rubio</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1747,13 +1747,13 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>23/09/1973</t>
+          <t>26/03/1969</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>3443 Cook Flat Suite 564
-Burtonview, NM 90567</t>
+          <t>2927 Richard Lane
+Larsonberg, CT 37839</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1763,7 +1763,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Someone edge carry.</t>
+          <t>Describe strategy.</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -1773,43 +1773,43 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Seantown</t>
+          <t>Cookemouth</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>Growth treatment us.</t>
+          <t>Heart particular TV.</t>
         </is>
       </c>
       <c r="J19" t="n">
-        <v>41</v>
+        <v>87</v>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>Present explain.</t>
+          <t>Trip source land.</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>Partner large.</t>
+          <t>Home current door.</t>
         </is>
       </c>
       <c r="M19" t="n">
-        <v>9124</v>
+        <v>6089</v>
       </c>
       <c r="N19" t="n">
-        <v>2341</v>
+        <v>6372</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>out</t>
+          <t>either</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Jason Steele</t>
+          <t>Justin Thomas</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1819,13 +1819,13 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>27/07/1981</t>
+          <t>01/07/1953</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>PSC 7514, Box 0057
-APO AP 43978</t>
+          <t>60593 Burgess Loaf Suite 886
+Bryanfurt, LA 99653</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1835,7 +1835,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Room this son music.</t>
+          <t>Meet method lose.</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -1845,43 +1845,43 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Cassandrastad</t>
+          <t>East Devin</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>Traditional similar.</t>
+          <t>Finish century.</t>
         </is>
       </c>
       <c r="J20" t="n">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>Head performance.</t>
+          <t>Age part these.</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>Staff action any.</t>
+          <t>Open difference.</t>
         </is>
       </c>
       <c r="M20" t="n">
-        <v>3494</v>
+        <v>8601</v>
       </c>
       <c r="N20" t="n">
-        <v>3591</v>
+        <v>5530</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>appear</t>
+          <t>whether</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Melinda Wagner</t>
+          <t>Brent Brock</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1891,13 +1891,13 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>09/06/1985</t>
+          <t>02/03/1960</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>446 Sarah Cliffs Apt. 747
-South Barrymouth, NH 24239</t>
+          <t>USNV Watson
+FPO AP 92112</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1907,7 +1907,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Kitchen up left.</t>
+          <t>Player including.</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -1917,43 +1917,43 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>New Robert</t>
+          <t>Lake Kevin</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>Dream imagine town.</t>
+          <t>Recently far.</t>
         </is>
       </c>
       <c r="J21" t="n">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>Serve amount large.</t>
+          <t>Far old positive.</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>Certainly plan oil.</t>
+          <t>Half show hotel but.</t>
         </is>
       </c>
       <c r="M21" t="n">
-        <v>4138</v>
+        <v>3081</v>
       </c>
       <c r="N21" t="n">
-        <v>3388</v>
+        <v>3381</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>hope</t>
+          <t>trade</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Logan Lambert</t>
+          <t>Victoria Gibson</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1963,13 +1963,13 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>11/03/2002</t>
+          <t>24/07/1947</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>397 Bender Harbors
-Curtisfurt, IL 48756</t>
+          <t>989 Kevin Courts Suite 628
+Fletcherton, PA 98373</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1979,7 +1979,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Fly five meeting.</t>
+          <t>Perhaps cold wide.</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -1989,43 +1989,43 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Lake Paul</t>
+          <t>Port Andrew</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>Similar doctor.</t>
+          <t>Tree should late.</t>
         </is>
       </c>
       <c r="J22" t="n">
-        <v>38</v>
+        <v>79</v>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>Seven shoulder bag.</t>
+          <t>Relate reason.</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>Energy want often.</t>
+          <t>Trial create.</t>
         </is>
       </c>
       <c r="M22" t="n">
-        <v>4645</v>
+        <v>6781</v>
       </c>
       <c r="N22" t="n">
-        <v>5172</v>
+        <v>2535</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>before</t>
+          <t>deal</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Brenda Daniels</t>
+          <t>Jennifer Gibson</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -2035,13 +2035,13 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>20/09/1996</t>
+          <t>13/04/1943</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>9177 Craig Ports
-Matthewmouth, GA 24780</t>
+          <t>PSC 3551, Box 2374
+APO AA 07967</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -2051,7 +2051,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Part interesting.</t>
+          <t>Watch feel draw.</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -2061,43 +2061,43 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Saunderstown</t>
+          <t>North Angelaburgh</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>Structure never.</t>
+          <t>Action.</t>
         </is>
       </c>
       <c r="J23" t="n">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>Free test above.</t>
+          <t>Coach treatment.</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Cup feel continue.</t>
+          <t>Past base skill.</t>
         </is>
       </c>
       <c r="M23" t="n">
-        <v>3768</v>
+        <v>2447</v>
       </c>
       <c r="N23" t="n">
-        <v>5713</v>
+        <v>3602</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>final</t>
+          <t>skill</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Angelica Johnson</t>
+          <t>Thomas Peters</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -2107,13 +2107,13 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>02/12/1978</t>
+          <t>24/03/1935</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>68189 Melissa Fork
-Jenniferborough, AR 15848</t>
+          <t>2402 Brandon Cliff
+Port Kellyborough, CA 60361</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -2123,7 +2123,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Story for political.</t>
+          <t>Organization piece.</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -2133,43 +2133,43 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Lawrenceborough</t>
+          <t>Georgeport</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>Store street health.</t>
+          <t>The relate from.</t>
         </is>
       </c>
       <c r="J24" t="n">
-        <v>70</v>
+        <v>42</v>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>Through enough use.</t>
+          <t>Role recognize onto.</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Him toward better.</t>
+          <t>Great ask future.</t>
         </is>
       </c>
       <c r="M24" t="n">
-        <v>9791</v>
+        <v>3293</v>
       </c>
       <c r="N24" t="n">
-        <v>4808</v>
+        <v>1702</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>follow</t>
+          <t>foot</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Ashley Johnson MD</t>
+          <t>Aaron Smith</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -2179,13 +2179,13 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>05/06/2001</t>
+          <t>07/07/1956</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>71875 Ortega Bypass Suite 705
-Byrdstad, FL 88627</t>
+          <t>00336 Donald Station Suite 067
+Powellstad, OK 47233</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -2195,7 +2195,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Add call sell store.</t>
+          <t>Eight help task.</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -2205,43 +2205,43 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Sweeneybury</t>
+          <t>Lauraton</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>Man discover each.</t>
+          <t>Figure away vote.</t>
         </is>
       </c>
       <c r="J25" t="n">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>Box official.</t>
+          <t>Role enough middle.</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Yard difference.</t>
+          <t>Pretty gun now low.</t>
         </is>
       </c>
       <c r="M25" t="n">
-        <v>4926</v>
+        <v>9147</v>
       </c>
       <c r="N25" t="n">
-        <v>5617</v>
+        <v>2430</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>discuss</t>
+          <t>talk</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Travis Thomas</t>
+          <t>Sarah Cooper</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -2251,13 +2251,13 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>02/10/1948</t>
+          <t>27/01/1962</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>6023 Jacqueline Ridge Suite 053
-West Philip, KY 02197</t>
+          <t>USNV Hall
+FPO AE 68993</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -2267,7 +2267,7 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Mind beyond huge by.</t>
+          <t>Building represent.</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -2277,43 +2277,43 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Port David</t>
+          <t>Rebeccaside</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>Walk goal night.</t>
+          <t>The decide and.</t>
         </is>
       </c>
       <c r="J26" t="n">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>News information.</t>
+          <t>Recently air author.</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>Economy generation.</t>
+          <t>Population price.</t>
         </is>
       </c>
       <c r="M26" t="n">
-        <v>7444</v>
+        <v>9617</v>
       </c>
       <c r="N26" t="n">
-        <v>5097</v>
+        <v>7995</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>practice</t>
+          <t>prepare</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Lindsey Robinson</t>
+          <t>Ian Woodard</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -2323,13 +2323,13 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>10/05/1930</t>
+          <t>15/01/2000</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>749 Howard Mews Suite 106
-South Colleenton, HI 45949</t>
+          <t>93952 Kirby Station Suite 917
+Deleonland, GU 71717</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -2339,7 +2339,7 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Environmental light.</t>
+          <t>Deal truth join.</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -2349,43 +2349,43 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>South Terrance</t>
+          <t>South Taylortown</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>Glass produce.</t>
+          <t>Source ready.</t>
         </is>
       </c>
       <c r="J27" t="n">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>Development fear.</t>
+          <t>Paper approach most.</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Live miss former.</t>
+          <t>Price ok according.</t>
         </is>
       </c>
       <c r="M27" t="n">
-        <v>4235</v>
+        <v>4581</v>
       </c>
       <c r="N27" t="n">
-        <v>2661</v>
+        <v>3230</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>game</t>
+          <t>mother</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Whitney Torres</t>
+          <t>Lucas Newton</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -2395,13 +2395,13 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>27/07/1934</t>
+          <t>26/04/1971</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>8669 Andersen Fall Suite 300
-East Brianna, GU 57511</t>
+          <t>1707 Chase Ways
+Hicksmouth, NJ 47962</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -2411,7 +2411,7 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Term attack them.</t>
+          <t>Building thing.</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
@@ -2421,43 +2421,43 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Lake Mario</t>
+          <t>Haleymouth</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>Around street boy.</t>
+          <t>The ago oil summer.</t>
         </is>
       </c>
       <c r="J28" t="n">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>Manager back myself.</t>
+          <t>Very remember.</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Mother show.</t>
+          <t>Four federal.</t>
         </is>
       </c>
       <c r="M28" t="n">
-        <v>5262</v>
+        <v>2590</v>
       </c>
       <c r="N28" t="n">
-        <v>1927</v>
+        <v>6765</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>open</t>
+          <t>watch</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Nicolas Underwood</t>
+          <t>Kimberly Rowland</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -2467,13 +2467,13 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>12/07/1965</t>
+          <t>13/06/1956</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>5141 Flores Points
-North Douglas, IL 38025</t>
+          <t>02875 Neal Isle
+Mcdonaldshire, PA 30325</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -2483,7 +2483,7 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Worry doctor his.</t>
+          <t>Put possible fine.</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
@@ -2493,43 +2493,43 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Sandovalberg</t>
+          <t>North Kelsey</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>Goal political trip.</t>
+          <t>Level sister.</t>
         </is>
       </c>
       <c r="J29" t="n">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>Model specific now.</t>
+          <t>Put between various.</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>But about pass.</t>
+          <t>Wind tree hold.</t>
         </is>
       </c>
       <c r="M29" t="n">
-        <v>5078</v>
+        <v>5641</v>
       </c>
       <c r="N29" t="n">
-        <v>3317</v>
+        <v>4768</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>national</t>
+          <t>factor</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Cody Farrell</t>
+          <t>Anthony Garner</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -2539,13 +2539,13 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>08/02/1928</t>
+          <t>16/01/1986</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>144 Ricardo Vista Apt. 480
-Dixontown, VI 35294</t>
+          <t>52578 Molina Ferry Suite 364
+West Daniellechester, ND 41899</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -2555,7 +2555,7 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Soldier lead behind.</t>
+          <t>Method bad free.</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -2565,43 +2565,43 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>New Melissaburgh</t>
+          <t>New Sheila</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>Realize teach those.</t>
+          <t>Time above natural.</t>
         </is>
       </c>
       <c r="J30" t="n">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>Itself wish top.</t>
+          <t>Hotel all difficult.</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>True item any media.</t>
+          <t>More side young.</t>
         </is>
       </c>
       <c r="M30" t="n">
-        <v>6188</v>
+        <v>6250</v>
       </c>
       <c r="N30" t="n">
-        <v>4625</v>
+        <v>3666</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>benefit</t>
+          <t>ability</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Michael Wright</t>
+          <t>Allen Alvarez</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -2611,13 +2611,13 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>09/06/1995</t>
+          <t>26/06/1939</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>100 Hurley Island Apt. 812
-Hoffmanbury, NC 14561</t>
+          <t>72493 Sandy Prairie Apt. 059
+East Dawn, LA 63121</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -2627,7 +2627,7 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Ten language affect.</t>
+          <t>Reality successful.</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
@@ -2637,36 +2637,36 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>North Karaborough</t>
+          <t>North Ryanstad</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>Section boy who.</t>
+          <t>Pull cultural along.</t>
         </is>
       </c>
       <c r="J31" t="n">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>Most keep.</t>
+          <t>Base his next.</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>Music field.</t>
+          <t>Important help.</t>
         </is>
       </c>
       <c r="M31" t="n">
-        <v>9273</v>
+        <v>2191</v>
       </c>
       <c r="N31" t="n">
-        <v>9273</v>
+        <v>4326</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>hard</t>
+          <t>magazine</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Enhanced the masking techniques
</commit_message>
<xml_diff>
--- a/backend/uploads/masked/masked_Student_Information.xlsx
+++ b/backend/uploads/masked/masked_Student_Information.xlsx
@@ -513,23 +513,23 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Lisa Adams</t>
+          <t>Jasmine Day</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>9**********4</t>
+          <t>3************2</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>19/02/1995</t>
+          <t>28/09/1933</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>29005 Bryan Heights
-Port Sarahhaven, DE 77487</t>
+          <t>95604 Cassandra Road Apt. 633
+Port Victoriafort, CO 71069</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -539,7 +539,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>The meeting myself.</t>
+          <t>Perform address.</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -549,59 +549,59 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>South Shannon</t>
+          <t>North Jacob</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Size one health he.</t>
+          <t>No up citizen when.</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>77</v>
+        <v>47</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Partner too risk.</t>
+          <t>State including.</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Truth view score.</t>
+          <t>Determine her.</t>
         </is>
       </c>
       <c r="M2" t="n">
-        <v>2053</v>
+        <v>3948</v>
       </c>
       <c r="N2" t="n">
-        <v>6377</v>
+        <v>9633</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>standard</t>
+          <t>shake</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Sandra Rogers</t>
+          <t>Chris Villegas</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>9**********5</t>
+          <t>8************5</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>29/01/1999</t>
+          <t>14/01/1964</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>9244 Franklin Oval Apt. 569
-Michealborough, IL 45211</t>
+          <t>356 Townsend Islands
+Lake Matthew, NJ 15801</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -611,7 +611,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Alone tell support.</t>
+          <t>Theory move.</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -621,59 +621,59 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Lake Lori</t>
+          <t>East Henry</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Wrong newspaper per.</t>
+          <t>Enter sometimes PM.</t>
         </is>
       </c>
       <c r="J3" t="n">
-        <v>35</v>
+        <v>90</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Democrat fly people.</t>
+          <t>Born political use.</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Difficult data.</t>
+          <t>Mention before list.</t>
         </is>
       </c>
       <c r="M3" t="n">
-        <v>4599</v>
+        <v>2016</v>
       </c>
       <c r="N3" t="n">
-        <v>2124</v>
+        <v>3598</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>vote</t>
+          <t>offer</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Jason Hogan</t>
+          <t>Donna Walsh</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>9**********6</t>
+          <t>8************6</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>05/03/2005</t>
+          <t>16/09/1976</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Unit 8170 Box 4535
-DPO AP 31029</t>
+          <t>5040 Bryant Motorway
+West Janet, IA 23729</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -683,7 +683,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Consider reflect.</t>
+          <t>Nor rich debate.</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -693,59 +693,59 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>New Brookefort</t>
+          <t>North Codychester</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Parent contain ago.</t>
+          <t>Body treatment.</t>
         </is>
       </c>
       <c r="J4" t="n">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Leave son market.</t>
+          <t>Subject human.</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Pay which mention.</t>
+          <t>Yeah when product.</t>
         </is>
       </c>
       <c r="M4" t="n">
-        <v>8454</v>
+        <v>8352</v>
       </c>
       <c r="N4" t="n">
-        <v>1011</v>
+        <v>4204</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>something</t>
+          <t>animal</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Diana Owens</t>
+          <t>Ian Vasquez DDS</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>9**********7</t>
+          <t>4************8</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>23/12/1958</t>
+          <t>01/08/1933</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>711 Kellie Road
-South Jason, OH 41719</t>
+          <t>233 Zachary Course Apt. 717
+Perryborough, WA 82106</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -755,7 +755,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Carry citizen chair.</t>
+          <t>Over position.</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -765,59 +765,59 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>New Sherryshire</t>
+          <t>Matthewhaven</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Hotel cup project.</t>
+          <t>Of room measure.</t>
         </is>
       </c>
       <c r="J5" t="n">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Somebody own.</t>
+          <t>Congress move begin.</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>Light these teach.</t>
+          <t>No method start.</t>
         </is>
       </c>
       <c r="M5" t="n">
-        <v>2195</v>
+        <v>2642</v>
       </c>
       <c r="N5" t="n">
-        <v>1197</v>
+        <v>6425</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>lot</t>
+          <t>work</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Stuart Santiago</t>
+          <t>Alex Russell</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>9**********8</t>
+          <t>6************6</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>19/10/1957</t>
+          <t>18/01/1927</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>USS Guzman
-FPO AA 39720</t>
+          <t>144 Brett Park Suite 101
+Lake Christopher, MD 55636</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -827,7 +827,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Agency call but.</t>
+          <t>Officer yourself.</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -837,59 +837,59 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Adriantown</t>
+          <t>Gonzalesmouth</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Head through.</t>
+          <t>Beyond language.</t>
         </is>
       </c>
       <c r="J6" t="n">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Wall sport free air.</t>
+          <t>By rich training.</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>Race myself fish.</t>
+          <t>Cost should second.</t>
         </is>
       </c>
       <c r="M6" t="n">
-        <v>2921</v>
+        <v>4940</v>
       </c>
       <c r="N6" t="n">
-        <v>9787</v>
+        <v>9056</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>about</t>
+          <t>will</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Jeffrey Holloway</t>
+          <t>Jason Elliott</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>9**********9</t>
+          <t>7************8</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>24/02/1942</t>
+          <t>02/06/1947</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>439 Wendy Via
-Lisahaven, UT 17632</t>
+          <t>USCGC Carlson
+FPO AA 19018</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -899,7 +899,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Wonder fast.</t>
+          <t>News social list.</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -909,59 +909,59 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>New Julia</t>
+          <t>Lake Matthewberg</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Again use key store.</t>
+          <t>Only maybe history.</t>
         </is>
       </c>
       <c r="J7" t="n">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Be position.</t>
+          <t>Wrong our article.</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Make style figure.</t>
+          <t>Local strategy.</t>
         </is>
       </c>
       <c r="M7" t="n">
-        <v>7749</v>
+        <v>3499</v>
       </c>
       <c r="N7" t="n">
-        <v>8018</v>
+        <v>7904</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>administration</t>
+          <t>live</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Nicholas Mitchell</t>
+          <t>John Collins</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>9**********0</t>
+          <t>8************0</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>02/02/1993</t>
+          <t>31/08/1933</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>204 Cole Plains
-Port Justin, MS 95954</t>
+          <t>2189 Martin Street
+North Amanda, GU 59555</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -971,7 +971,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Skin white.</t>
+          <t>Various oil what.</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -981,59 +981,59 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Port Nicoleland</t>
+          <t>Carpenterfurt</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>National side no.</t>
+          <t>Future able street.</t>
         </is>
       </c>
       <c r="J8" t="n">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Agent box specific.</t>
+          <t>Can difference term.</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>Interview floor.</t>
+          <t>Father decide key.</t>
         </is>
       </c>
       <c r="M8" t="n">
-        <v>7890</v>
+        <v>8112</v>
       </c>
       <c r="N8" t="n">
-        <v>8225</v>
+        <v>7459</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>individual</t>
+          <t>within</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Ricardo Davis</t>
+          <t>Erica Keller</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>9**********1</t>
+          <t>9************6</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>15/02/1986</t>
+          <t>20/08/1985</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>09863 Jessica Estates
-North Marc, VA 19730</t>
+          <t>853 Allen Plains Apt. 968
+Howardborough, IA 63954</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -1043,7 +1043,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Still partner next.</t>
+          <t>Daughter cause.</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -1053,59 +1053,59 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Charlesstad</t>
+          <t>East Amy</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Practice husband.</t>
+          <t>Room toward before.</t>
         </is>
       </c>
       <c r="J9" t="n">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Together collection.</t>
+          <t>Bag between leader.</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>Pretty cover.</t>
+          <t>Business economic.</t>
         </is>
       </c>
       <c r="M9" t="n">
-        <v>9308</v>
+        <v>2720</v>
       </c>
       <c r="N9" t="n">
-        <v>7326</v>
+        <v>5999</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>edge</t>
+          <t>behind</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Brett Scott</t>
+          <t>Jennifer Butler</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>0**********2</t>
+          <t>2************0</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>19/09/1967</t>
+          <t>17/12/1972</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Unit 8558 Box 3894
-DPO AP 85220</t>
+          <t>1259 Baker Parks Suite 277
+Burkeland, CO 62870</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -1115,7 +1115,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>State because.</t>
+          <t>Success green.</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -1125,59 +1125,59 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>South Sarah</t>
+          <t>Campbellfort</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Write sense note.</t>
+          <t>Ahead them fall.</t>
         </is>
       </c>
       <c r="J10" t="n">
-        <v>22</v>
+        <v>81</v>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Special bring hour.</t>
+          <t>Factor him cause.</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>Behind order stand.</t>
+          <t>Me camera shake.</t>
         </is>
       </c>
       <c r="M10" t="n">
-        <v>6035</v>
+        <v>4319</v>
       </c>
       <c r="N10" t="n">
-        <v>4074</v>
+        <v>3134</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>race</t>
+          <t>building</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Richard Howard</t>
+          <t>Linda Tran</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>0**********3</t>
+          <t>5************8</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>18/09/1993</t>
+          <t>02/01/1946</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>073 Robinson Unions Suite 180
-Hebertview, AS 83530</t>
+          <t>7114 Sanchez Canyon Suite 597
+Houstontown, IN 40676</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -1187,7 +1187,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Both hospital send.</t>
+          <t>Training attorney.</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -1197,59 +1197,59 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>East Craig</t>
+          <t>Kennethmouth</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Attorney front.</t>
+          <t>Officer me speak.</t>
         </is>
       </c>
       <c r="J11" t="n">
-        <v>88</v>
+        <v>62</v>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>Series chance may.</t>
+          <t>Much name protect.</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>Challenge structure.</t>
+          <t>Show moment.</t>
         </is>
       </c>
       <c r="M11" t="n">
-        <v>2042</v>
+        <v>3825</v>
       </c>
       <c r="N11" t="n">
-        <v>6804</v>
+        <v>6888</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>create</t>
+          <t>tree</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Drew Kane</t>
+          <t>Jessica Brown</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>0**********4</t>
+          <t>4************1</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>18/07/1946</t>
+          <t>19/02/1989</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>PSC 5825, Box 1127
-APO AE 53983</t>
+          <t>852 Darrell Estate
+Andrewborough, MN 37579</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -1259,7 +1259,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Street worry just.</t>
+          <t>Pull husband.</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -1269,59 +1269,59 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Port Michaelborough</t>
+          <t>East Megan</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>How group stuff.</t>
+          <t>Space tell suffer.</t>
         </is>
       </c>
       <c r="J12" t="n">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>Look heavy wonder.</t>
+          <t>Watch position.</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>Tough force early.</t>
+          <t>Human theory coach.</t>
         </is>
       </c>
       <c r="M12" t="n">
-        <v>4678</v>
+        <v>6394</v>
       </c>
       <c r="N12" t="n">
-        <v>2204</v>
+        <v>6384</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>phone</t>
+          <t>spend</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Yvonne Taylor</t>
+          <t>Tyler Wilkerson</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>0**********5</t>
+          <t>0************7</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>26/03/1942</t>
+          <t>20/01/1936</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>6254 Susan Plaza Apt. 256
-South Daniel, CT 46017</t>
+          <t>9455 Jeffrey Court Suite 350
+North Susanfurt, CT 30635</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -1331,7 +1331,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Outside sing save.</t>
+          <t>Relationship hit.</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -1341,59 +1341,59 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>East Lacey</t>
+          <t>South Carlland</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>Light dark letter.</t>
+          <t>Billion real.</t>
         </is>
       </c>
       <c r="J13" t="n">
-        <v>47</v>
+        <v>81</v>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Conference player.</t>
+          <t>Direction prove.</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>The remember them.</t>
+          <t>One dark democratic.</t>
         </is>
       </c>
       <c r="M13" t="n">
-        <v>2673</v>
+        <v>9039</v>
       </c>
       <c r="N13" t="n">
-        <v>5481</v>
+        <v>2401</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>style</t>
+          <t>majority</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Jose Rivera</t>
+          <t>Taylor Rowe</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>0**********6</t>
+          <t>5************3</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>27/02/1967</t>
+          <t>27/02/1974</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>28283 Williams Ford Apt. 175
-East Caleb, WA 75733</t>
+          <t>8452 Bennett River Suite 609
+West Heather, SC 96601</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1403,7 +1403,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Cell describe.</t>
+          <t>Record social every.</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -1413,59 +1413,59 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Francohaven</t>
+          <t>Davidburgh</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>Left mission lose.</t>
+          <t>Thousand oil sense.</t>
         </is>
       </c>
       <c r="J14" t="n">
-        <v>86</v>
+        <v>30</v>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>Item physical film.</t>
+          <t>Attorney recent.</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Charge above.</t>
+          <t>Before issue event.</t>
         </is>
       </c>
       <c r="M14" t="n">
-        <v>4381</v>
+        <v>6887</v>
       </c>
       <c r="N14" t="n">
-        <v>8882</v>
+        <v>9577</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>project</t>
+          <t>blue</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Kelly Harrison</t>
+          <t>Lindsey Stuart</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>0**********7</t>
+          <t>8************2</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>18/10/2002</t>
+          <t>27/04/1949</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>357 Deborah Lights
-Butlerfurt, MD 35339</t>
+          <t>55064 Munoz Meadows
+West Autumn, TX 49288</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1475,7 +1475,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Arrive rule within.</t>
+          <t>Away voice.</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -1485,59 +1485,59 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>South Kevin</t>
+          <t>South Teresastad</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>Focus thing ok.</t>
+          <t>Guess unit heart.</t>
         </is>
       </c>
       <c r="J15" t="n">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>It agreement stock.</t>
+          <t>Same great still.</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>Dog might daughter.</t>
+          <t>To under movie ask.</t>
         </is>
       </c>
       <c r="M15" t="n">
-        <v>6505</v>
+        <v>5929</v>
       </c>
       <c r="N15" t="n">
-        <v>3092</v>
+        <v>6438</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>measure</t>
+          <t>group</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Frank Walker</t>
+          <t>Michael Butler</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>0**********8</t>
+          <t>5************1</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>23/01/1967</t>
+          <t>12/12/1977</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>032 Ruiz Landing
-East Zoechester, MN 26575</t>
+          <t>26513 Campbell Stravenue Apt. 183
+West Scottfort, UT 28555</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1547,7 +1547,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Yes nice us skin.</t>
+          <t>Outside best.</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1557,59 +1557,59 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>North Mike</t>
+          <t>Tiffanyview</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>Cover despite size.</t>
+          <t>Week part thank.</t>
         </is>
       </c>
       <c r="J16" t="n">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>Us forward style.</t>
+          <t>Rich scientist.</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>Word feel seem.</t>
+          <t>Manager almost.</t>
         </is>
       </c>
       <c r="M16" t="n">
-        <v>5854</v>
+        <v>5419</v>
       </c>
       <c r="N16" t="n">
-        <v>4999</v>
+        <v>6910</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>easy</t>
+          <t>role</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Dr. Gregory Bell</t>
+          <t>Vanessa Campos</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>0**********9</t>
+          <t>3************1</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>29/07/1974</t>
+          <t>24/07/1982</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>5091 James Roads Apt. 198
-Ashleyshire, IA 58448</t>
+          <t>86212 Johnson Ways Apt. 892
+Smithfort, ID 90278</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1619,7 +1619,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Trip spend page.</t>
+          <t>Girl require writer.</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1629,59 +1629,59 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Hensleyberg</t>
+          <t>East James</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>Environmental pull.</t>
+          <t>None speech.</t>
         </is>
       </c>
       <c r="J17" t="n">
-        <v>89</v>
+        <v>53</v>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>Help education.</t>
+          <t>Position best that.</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>Serve store tonight.</t>
+          <t>Ground teach short.</t>
         </is>
       </c>
       <c r="M17" t="n">
-        <v>5138</v>
+        <v>4849</v>
       </c>
       <c r="N17" t="n">
-        <v>8357</v>
+        <v>8887</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>cut</t>
+          <t>art</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>James Rangel</t>
+          <t>Timothy Moreno</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>0**********0</t>
+          <t>7************9</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>23/09/1969</t>
+          <t>24/05/2006</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>5316 Kimberly Lakes
-Brittanyville, AZ 35336</t>
+          <t>7518 Barbara Manors
+Timothymouth, OH 79682</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1691,7 +1691,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Wonder technology.</t>
+          <t>Position trip.</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -1701,59 +1701,59 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>West Timothyside</t>
+          <t>West Stevenstad</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>Writer join indeed.</t>
+          <t>Activity thank.</t>
         </is>
       </c>
       <c r="J18" t="n">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Serve life until.</t>
+          <t>Money kind reflect.</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>Mrs card remain.</t>
+          <t>Others work discuss.</t>
         </is>
       </c>
       <c r="M18" t="n">
-        <v>5712</v>
+        <v>8809</v>
       </c>
       <c r="N18" t="n">
-        <v>2088</v>
+        <v>9891</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>figure</t>
+          <t>offer</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Eric Rubio</t>
+          <t>Ashley Roach</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>0**********1</t>
+          <t>9************5</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>26/03/1969</t>
+          <t>17/04/1957</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2927 Richard Lane
-Larsonberg, CT 37839</t>
+          <t>0106 Henry Stravenue
+East Angela, NC 74149</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1763,7 +1763,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Describe strategy.</t>
+          <t>Wear growth system.</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -1773,59 +1773,59 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Cookemouth</t>
+          <t>Karenhaven</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>Heart particular TV.</t>
+          <t>Rate kitchen fish.</t>
         </is>
       </c>
       <c r="J19" t="n">
-        <v>87</v>
+        <v>45</v>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>Trip source land.</t>
+          <t>Rate meeting chair.</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>Home current door.</t>
+          <t>Quickly although.</t>
         </is>
       </c>
       <c r="M19" t="n">
-        <v>6089</v>
+        <v>2166</v>
       </c>
       <c r="N19" t="n">
-        <v>6372</v>
+        <v>4469</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>either</t>
+          <t>pretty</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Justin Thomas</t>
+          <t>Jenna Jones</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>1**********2</t>
+          <t>4************6</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>01/07/1953</t>
+          <t>23/07/1935</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>60593 Burgess Loaf Suite 886
-Bryanfurt, LA 99653</t>
+          <t>2895 Pacheco Ranch Apt. 824
+Simsborough, PA 31956</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1835,7 +1835,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Meet method lose.</t>
+          <t>Remember give.</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -1845,59 +1845,59 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>East Devin</t>
+          <t>North Donna</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>Finish century.</t>
+          <t>Make into card firm.</t>
         </is>
       </c>
       <c r="J20" t="n">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>Age part these.</t>
+          <t>Part wide current.</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>Open difference.</t>
+          <t>Pretty key.</t>
         </is>
       </c>
       <c r="M20" t="n">
-        <v>8601</v>
+        <v>9836</v>
       </c>
       <c r="N20" t="n">
-        <v>5530</v>
+        <v>6315</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>whether</t>
+          <t>remember</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Brent Brock</t>
+          <t>Ashley Hansen</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>1**********3</t>
+          <t>4************4</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>02/03/1960</t>
+          <t>23/06/1927</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>USNV Watson
-FPO AP 92112</t>
+          <t>USS Garcia
+FPO AA 51097</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1907,7 +1907,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Player including.</t>
+          <t>View join walk cell.</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -1917,59 +1917,59 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Lake Kevin</t>
+          <t>Byrdton</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>Recently far.</t>
+          <t>Second lot if hold.</t>
         </is>
       </c>
       <c r="J21" t="n">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>Far old positive.</t>
+          <t>Science management.</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>Half show hotel but.</t>
+          <t>Interest perform.</t>
         </is>
       </c>
       <c r="M21" t="n">
-        <v>3081</v>
+        <v>9461</v>
       </c>
       <c r="N21" t="n">
-        <v>3381</v>
+        <v>4164</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>trade</t>
+          <t>daughter</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Victoria Gibson</t>
+          <t>Emma Marshall</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>1**********4</t>
+          <t>4************3</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>24/07/1947</t>
+          <t>16/03/1944</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>989 Kevin Courts Suite 628
-Fletcherton, PA 98373</t>
+          <t>2579 Hall Lights
+Josephburgh, IN 92388</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1979,7 +1979,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Perhaps cold wide.</t>
+          <t>Daughter must upon.</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -1989,59 +1989,59 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Port Andrew</t>
+          <t>Andrewhaven</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>Tree should late.</t>
+          <t>Mean avoid itself.</t>
         </is>
       </c>
       <c r="J22" t="n">
-        <v>79</v>
+        <v>48</v>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>Relate reason.</t>
+          <t>Pay among human.</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>Trial create.</t>
+          <t>Woman budget sport.</t>
         </is>
       </c>
       <c r="M22" t="n">
-        <v>6781</v>
+        <v>6664</v>
       </c>
       <c r="N22" t="n">
-        <v>2535</v>
+        <v>4963</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>deal</t>
+          <t>firm</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Jennifer Gibson</t>
+          <t>Harry Wilson</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>1**********5</t>
+          <t>0************0</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>13/04/1943</t>
+          <t>09/12/2005</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>PSC 3551, Box 2374
-APO AA 07967</t>
+          <t>524 Jonathan Causeway Apt. 771
+Annehaven, MH 35480</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -2051,7 +2051,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Watch feel draw.</t>
+          <t>Cut who raise.</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -2061,59 +2061,59 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>North Angelaburgh</t>
+          <t>North Brittany</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>Action.</t>
+          <t>Say decision find.</t>
         </is>
       </c>
       <c r="J23" t="n">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>Coach treatment.</t>
+          <t>For surface stop.</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Past base skill.</t>
+          <t>Evening value him.</t>
         </is>
       </c>
       <c r="M23" t="n">
-        <v>2447</v>
+        <v>3063</v>
       </c>
       <c r="N23" t="n">
-        <v>3602</v>
+        <v>8773</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>skill</t>
+          <t>yeah</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Thomas Peters</t>
+          <t>Patricia Kramer</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>1**********6</t>
+          <t>7************0</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>24/03/1935</t>
+          <t>24/10/1979</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>2402 Brandon Cliff
-Port Kellyborough, CA 60361</t>
+          <t>78667 Jeffrey Grove
+Lake Marissachester, RI 23908</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -2123,7 +2123,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Organization piece.</t>
+          <t>Mean total state.</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -2133,59 +2133,59 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Georgeport</t>
+          <t>North Coleshire</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>The relate from.</t>
+          <t>Through try skill.</t>
         </is>
       </c>
       <c r="J24" t="n">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>Role recognize onto.</t>
+          <t>Subject record.</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Great ask future.</t>
+          <t>Page wish meet my.</t>
         </is>
       </c>
       <c r="M24" t="n">
-        <v>3293</v>
+        <v>6323</v>
       </c>
       <c r="N24" t="n">
-        <v>1702</v>
+        <v>6877</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>foot</t>
+          <t>shoulder</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Aaron Smith</t>
+          <t>Kaitlin Brennan</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>1**********7</t>
+          <t>0************2</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>07/07/1956</t>
+          <t>13/08/1975</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>00336 Donald Station Suite 067
-Powellstad, OK 47233</t>
+          <t>973 Gardner Hollow
+Ballchester, FM 35574</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -2195,7 +2195,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Eight help task.</t>
+          <t>Agent nice voice.</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -2205,59 +2205,59 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Lauraton</t>
+          <t>East Frank</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>Figure away vote.</t>
+          <t>Forget imagine.</t>
         </is>
       </c>
       <c r="J25" t="n">
-        <v>24</v>
+        <v>70</v>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>Role enough middle.</t>
+          <t>Laugh industry.</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Pretty gun now low.</t>
+          <t>Happy standard.</t>
         </is>
       </c>
       <c r="M25" t="n">
-        <v>9147</v>
+        <v>8758</v>
       </c>
       <c r="N25" t="n">
-        <v>2430</v>
+        <v>8357</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>talk</t>
+          <t>process</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Sarah Cooper</t>
+          <t>Molly Mcknight</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>1**********8</t>
+          <t>7************4</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>27/01/1962</t>
+          <t>31/08/1966</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>USNV Hall
-FPO AE 68993</t>
+          <t>27667 Gates Cove Suite 107
+Nicolefort, TX 33737</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -2267,7 +2267,7 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Building represent.</t>
+          <t>Production sense.</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -2277,59 +2277,59 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Rebeccaside</t>
+          <t>New Keith</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>The decide and.</t>
+          <t>Recognize challenge.</t>
         </is>
       </c>
       <c r="J26" t="n">
-        <v>66</v>
+        <v>25</v>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>Recently air author.</t>
+          <t>Outside reflect.</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>Population price.</t>
+          <t>Begin one anything.</t>
         </is>
       </c>
       <c r="M26" t="n">
-        <v>9617</v>
+        <v>8511</v>
       </c>
       <c r="N26" t="n">
-        <v>7995</v>
+        <v>7165</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>prepare</t>
+          <t>community</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Ian Woodard</t>
+          <t>Jennifer Castro</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>1**********9</t>
+          <t>4************0</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>15/01/2000</t>
+          <t>08/02/1974</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>93952 Kirby Station Suite 917
-Deleonland, GU 71717</t>
+          <t>78506 Nicole Cliff
+Port Kevinborough, TN 06706</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -2339,7 +2339,7 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Deal truth join.</t>
+          <t>Save bank TV.</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -2349,59 +2349,59 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>South Taylortown</t>
+          <t>Port Gregory</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>Source ready.</t>
+          <t>Social method.</t>
         </is>
       </c>
       <c r="J27" t="n">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>Paper approach most.</t>
+          <t>Rich or firm.</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Price ok according.</t>
+          <t>Anything body.</t>
         </is>
       </c>
       <c r="M27" t="n">
-        <v>4581</v>
+        <v>4941</v>
       </c>
       <c r="N27" t="n">
-        <v>3230</v>
+        <v>5423</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>mother</t>
+          <t>though</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Lucas Newton</t>
+          <t>Cheryl Lee</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>1**********0</t>
+          <t>4************0</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>26/04/1971</t>
+          <t>19/05/1972</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1707 Chase Ways
-Hicksmouth, NJ 47962</t>
+          <t>7825 West Forest
+East Jason, KS 35208</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -2411,7 +2411,7 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Building thing.</t>
+          <t>Simple fine often.</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
@@ -2421,59 +2421,59 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Haleymouth</t>
+          <t>Lindsayview</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>The ago oil summer.</t>
+          <t>Share listen.</t>
         </is>
       </c>
       <c r="J28" t="n">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>Very remember.</t>
+          <t>International need.</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Four federal.</t>
+          <t>Lead forget six.</t>
         </is>
       </c>
       <c r="M28" t="n">
-        <v>2590</v>
+        <v>3895</v>
       </c>
       <c r="N28" t="n">
-        <v>6765</v>
+        <v>8207</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>watch</t>
+          <t>ability</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Kimberly Rowland</t>
+          <t>Ryan Brown</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>1**********1</t>
+          <t>5************5</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>13/06/1956</t>
+          <t>17/11/1986</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>02875 Neal Isle
-Mcdonaldshire, PA 30325</t>
+          <t>115 Cardenas Mountain Suite 333
+Christinamouth, LA 83337</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -2483,7 +2483,7 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Put possible fine.</t>
+          <t>Play full team.</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
@@ -2493,59 +2493,59 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>North Kelsey</t>
+          <t>North Coryview</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>Level sister.</t>
+          <t>Fill culture read.</t>
         </is>
       </c>
       <c r="J29" t="n">
-        <v>54</v>
+        <v>19</v>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>Put between various.</t>
+          <t>Hope into social.</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Wind tree hold.</t>
+          <t>Remember option.</t>
         </is>
       </c>
       <c r="M29" t="n">
-        <v>5641</v>
+        <v>9140</v>
       </c>
       <c r="N29" t="n">
-        <v>4768</v>
+        <v>8056</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>factor</t>
+          <t>accept</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Anthony Garner</t>
+          <t>Jennifer Heath</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>2**********2</t>
+          <t>2************0</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>16/01/1986</t>
+          <t>09/10/1935</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>52578 Molina Ferry Suite 364
-West Daniellechester, ND 41899</t>
+          <t>5778 Burgess Stravenue
+Port Patriciaside, PA 48083</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -2555,7 +2555,7 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Method bad free.</t>
+          <t>Anyone mother.</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -2565,59 +2565,59 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>New Sheila</t>
+          <t>East James</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>Time above natural.</t>
+          <t>Position challenge.</t>
         </is>
       </c>
       <c r="J30" t="n">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>Hotel all difficult.</t>
+          <t>Chair statement no.</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>More side young.</t>
+          <t>Stand federal final.</t>
         </is>
       </c>
       <c r="M30" t="n">
-        <v>6250</v>
+        <v>9582</v>
       </c>
       <c r="N30" t="n">
-        <v>3666</v>
+        <v>7280</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>ability</t>
+          <t>over</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Allen Alvarez</t>
+          <t>Holly Torres</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>2**********3</t>
+          <t>7************3</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>26/06/1939</t>
+          <t>14/07/1974</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>72493 Sandy Prairie Apt. 059
-East Dawn, LA 63121</t>
+          <t>PSC 7807, Box 0960
+APO AA 28266</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -2627,7 +2627,7 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Reality successful.</t>
+          <t>Large recently let.</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
@@ -2637,36 +2637,36 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>North Ryanstad</t>
+          <t>Kaylaborough</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>Pull cultural along.</t>
+          <t>Condition billion.</t>
         </is>
       </c>
       <c r="J31" t="n">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>Base his next.</t>
+          <t>Think plant space.</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>Important help.</t>
+          <t>Black TV everything.</t>
         </is>
       </c>
       <c r="M31" t="n">
-        <v>2191</v>
+        <v>7819</v>
       </c>
       <c r="N31" t="n">
-        <v>4326</v>
+        <v>3449</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>magazine</t>
+          <t>inside</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Finalized the masking techniques
</commit_message>
<xml_diff>
--- a/backend/uploads/masked/masked_Student_Information.xlsx
+++ b/backend/uploads/masked/masked_Student_Information.xlsx
@@ -513,28 +513,28 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>T*****y M****n</t>
+          <t>J***e L**e</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>5************5</t>
+          <t>9************7</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>17/08/1996</t>
+          <t>09/03/1975</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>* Dana Overpass
-North Jeanetteberg, GU *</t>
+          <t>* Erik Cliff Apt. *
+East Edward, KY *</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>(017)-*****02</t>
+          <t>(015)-*****94</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -544,22 +544,22 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>m**********n@example.net</t>
+          <t>d********7@example.net</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>P***k</t>
+          <t>P****s</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Healthy</t>
+          <t>Under Observation</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>40-49</t>
+          <t>50-59</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -574,43 +574,45 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>9000-9999</t>
-        </is>
-      </c>
-      <c r="N2" t="n">
-        <v>9307</v>
+          <t>13000-13999</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>*****</t>
+        </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>Church move cell.</t>
+          <t>*****</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>C*******e T****s</t>
+          <t>B*****a D***s</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>8************4</t>
+          <t>5************9</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>06/06/1928</t>
+          <t>16/04/1960</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>* Matthew Alley Apt. *
-East Lindseyburgh, KS *</t>
+          <t>* Freeman Junctions
+Lake Christineview, NC *</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>(010)-*****93</t>
+          <t>(012)-*****82</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -620,22 +622,22 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>w*********l@example.com</t>
+          <t>j******s@example.com</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>K***h</t>
+          <t>P****s</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Healthy</t>
+          <t>Under Observation</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>30-39</t>
+          <t>70-79</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -650,43 +652,45 @@
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>6000-6999</t>
-        </is>
-      </c>
-      <c r="N3" t="n">
-        <v>9458</v>
+          <t>12000-12999</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>*****</t>
+        </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Meet would.</t>
+          <t>*****</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>C*******e C***k</t>
+          <t>E**n J*****n</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>0************3</t>
+          <t>6************2</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>15/06/1961</t>
+          <t>13/03/1993</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>* Sierra Route
-Ninachester, OR *</t>
+          <t>* John Roads Suite *
+New Brianberg, MD *</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>(014)-*****72</t>
+          <t>(017)-*****94</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -696,22 +700,22 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>e**********n@example.org</t>
+          <t>a**********r@example.net</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>J****************m</t>
+          <t>M*****a</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Needs Attention</t>
+          <t>Healthy</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>50-59</t>
+          <t>90-99</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -726,43 +730,45 @@
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>12000-12999</t>
-        </is>
-      </c>
-      <c r="N4" t="n">
-        <v>6441</v>
+          <t>3000-3999</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>*****</t>
+        </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Mrs morning wear we.</t>
+          <t>*****</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>M******e G*******z</t>
+          <t>M*****l D*****n</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>0************2</t>
+          <t>8************0</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>04/08/1974</t>
+          <t>19/05/1987</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>* Allen Freeway Apt. *
-West Ryanhaven, PW *</t>
+          <t>* *
+FPO AE *</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>(013)-*****79</t>
+          <t>(012)-*****10</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -772,22 +778,22 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>b*******h@example.org</t>
+          <t>c******a@example.org</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>K**********r</t>
+          <t>S******r</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Needs Attention</t>
+          <t>Under Observation</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>50-59</t>
+          <t>20-29</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -802,43 +808,45 @@
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>3000-3999</t>
-        </is>
-      </c>
-      <c r="N5" t="n">
-        <v>6414</v>
+          <t>7000-7999</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>*****</t>
+        </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>Site stay physical.</t>
+          <t>*****</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>G**y M***s</t>
+          <t>A****y W****n</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>9************1</t>
+          <t>4************0</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>01/11/1948</t>
+          <t>27/01/1952</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>* Robbins Spur
-Garciachester, NV *</t>
+          <t>* Gonzalez Springs Apt. *
+Lake Stephaniefort, OR *</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>(016)-*****35</t>
+          <t>(010)-*****17</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -848,22 +856,22 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>s*****1@example.org</t>
+          <t>x******n@example.net</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>M*****a</t>
+          <t>T********u</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Critical</t>
+          <t>Needs Attention</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>90-99</t>
+          <t>30-39</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -878,43 +886,45 @@
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>5000-5999</t>
-        </is>
-      </c>
-      <c r="N6" t="n">
-        <v>5655</v>
+          <t>3000-3999</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>*****</t>
+        </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>Television tree.</t>
+          <t>*****</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>M****a D***s</t>
+          <t>E**c F****r</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>0************5</t>
+          <t>5************1</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>26/07/1930</t>
+          <t>08/07/1990</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>* Alicia Isle
-South Brettside, NV *</t>
+          <t>Unit * Box *
+DPO AP *</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>(011)-*****77</t>
+          <t>(012)-*****41</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -924,22 +934,22 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>b*******6@example.com</t>
+          <t>w*********y@example.net</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>K**********r</t>
+          <t>J****************m</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Under Observation</t>
+          <t>Needs Attention</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>90-99</t>
+          <t>50-59</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
@@ -954,43 +964,45 @@
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>3000-3999</t>
-        </is>
-      </c>
-      <c r="N7" t="n">
-        <v>9124</v>
+          <t>7000-7999</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>*****</t>
+        </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Gas also say part.</t>
+          <t>*****</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>D***a P****r</t>
+          <t>J***d T******n</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>7************1</t>
+          <t>3************9</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>18/10/1982</t>
+          <t>25/04/1936</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>* Murphy Inlet Suite *
-Christopherborough, GA *</t>
+          <t>Unit * Box *
+DPO AP *</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>(012)-*****49</t>
+          <t>(016)-*****32</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1000,17 +1012,17 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>c*********1@example.com</t>
+          <t>l****1@example.com</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>K******n</t>
+          <t>J****************m</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Critical</t>
+          <t>Recovering</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -1030,43 +1042,45 @@
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>5000-5999</t>
-        </is>
-      </c>
-      <c r="N8" t="n">
-        <v>9159</v>
+          <t>2000-2999</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>*****</t>
+        </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Even drop positive.</t>
+          <t>*****</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>A*****y D*****s</t>
+          <t>A****a D**n</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>7************0</t>
+          <t>7************3</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>06/03/1931</t>
+          <t>18/01/1945</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>* Rose Port Suite *
-Phillipsstad, AZ *</t>
+          <t>* Nelson Inlet Suite *
+Steventown, WI *</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>(012)-*****93</t>
+          <t>(018)-*****94</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1076,22 +1090,22 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>d*******1@example.org</t>
+          <t>l**********n@example.net</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>M*****a</t>
+          <t>S***h</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Recovering</t>
+          <t>Under Observation</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>30-39</t>
+          <t>50-59</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -1106,43 +1120,45 @@
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>8000-8999</t>
-        </is>
-      </c>
-      <c r="N9" t="n">
-        <v>4104</v>
+          <t>11000-11999</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>*****</t>
+        </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Thousand son.</t>
+          <t>*****</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>L**i B****s</t>
+          <t>N***y B*****t</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>9************0</t>
+          <t>8************7</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>27/11/1976</t>
+          <t>17/07/1949</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>* James Forge
-Lake Todd, VA *</t>
+          <t>* *
+FPO AP *</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>(017)-*****33</t>
+          <t>(018)-*****08</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1152,7 +1168,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>t*******4@example.com</t>
+          <t>b*****5@example.net</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -1162,12 +1178,12 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Needs Attention</t>
+          <t>Healthy</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>18-19</t>
+          <t>50-59</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
@@ -1182,43 +1198,45 @@
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>11000-11999</t>
-        </is>
-      </c>
-      <c r="N10" t="n">
-        <v>1150</v>
+          <t>8000-8999</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>*****</t>
+        </is>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Total truth.</t>
+          <t>*****</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>A****y R******s</t>
+          <t>K***n C*******s</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>4************4</t>
+          <t>6************4</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>05/01/1993</t>
+          <t>05/09/1978</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>PSC *, Box *
-APO AP *</t>
+          <t>* Jennifer Fall
+Jimenezburgh, NE *</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>(017)-*****04</t>
+          <t>(017)-*****43</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1228,22 +1246,22 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>v********5@example.com</t>
+          <t>c*******0@example.com</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>S*****k</t>
+          <t>P***k</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Healthy</t>
+          <t>Recovering</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>70-79</t>
+          <t>100-100</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
@@ -1258,43 +1276,45 @@
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>10000-10999</t>
-        </is>
-      </c>
-      <c r="N11" t="n">
-        <v>3745</v>
+          <t>6000-6999</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>*****</t>
+        </is>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Morning enjoy.</t>
+          <t>*****</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>B***n H***h</t>
+          <t>J***n B****s</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>4************6</t>
+          <t>3************9</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>16/01/1955</t>
+          <t>31/07/1977</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>* Joseph Parks Apt. *
-East Michelle, AZ *</t>
+          <t>* Jessica Summit
+Weberhaven, WI *</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>(010)-*****53</t>
+          <t>(011)-*****81</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1304,7 +1324,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>d*******0@example.com</t>
+          <t>s*********t@example.net</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -1314,12 +1334,12 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>Under Observation</t>
+          <t>Critical</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>80-89</t>
+          <t>20-29</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
@@ -1334,43 +1354,45 @@
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>3000-3999</t>
-        </is>
-      </c>
-      <c r="N12" t="n">
-        <v>4971</v>
+          <t>12000-12999</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>*****</t>
+        </is>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Ready fear apply.</t>
+          <t>*****</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>J**n P****e</t>
+          <t>M**. S**a J*****n</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>3************8</t>
+          <t>9************0</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>31/01/1946</t>
+          <t>10/08/2005</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>* Weber Stream
-Alvarezport, IL *</t>
+          <t>* Zimmerman Park Suite *
+South Brad, PW *</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>(013)-*****59</t>
+          <t>(010)-*****28</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1380,17 +1402,17 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>u*****x@example.net</t>
+          <t>j*******t@example.org</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>P****g</t>
+          <t>K***h</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>Needs Attention</t>
+          <t>Under Observation</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
@@ -1410,43 +1432,45 @@
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>3000-3999</t>
-        </is>
-      </c>
-      <c r="N13" t="n">
-        <v>8670</v>
+          <t>11000-11999</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>*****</t>
+        </is>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Media several up.</t>
+          <t>*****</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>R*****d W****r</t>
+          <t>R****t W**f</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>5************1</t>
+          <t>9************8</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>14/01/1958</t>
+          <t>10/05/1989</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>* Marissa Courts Apt. *
-Lake Samantha, LA *</t>
+          <t>* Morgan Curve
+Lake Meghanland, OK *</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>(011)-*****11</t>
+          <t>(019)-*****28</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1456,22 +1480,22 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>k******d@example.com</t>
+          <t>j*****7@example.com</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>S***h</t>
+          <t>T********u</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>Needs Attention</t>
+          <t>Under Observation</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>20-29</t>
+          <t>60-69</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -1486,43 +1510,45 @@
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>8000-8999</t>
-        </is>
-      </c>
-      <c r="N14" t="n">
-        <v>8626</v>
+          <t>12000-12999</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>*****</t>
+        </is>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Meet door shake.</t>
+          <t>*****</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>J**n R**e</t>
+          <t>J**n C***e</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>4************1</t>
+          <t>9************4</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>07/02/2000</t>
+          <t>15/11/1997</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>* Jessica Trail
-Victoriaport, AL *</t>
+          <t>* Sanchez Plain Suite *
+Julieport, MS *</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>(014)-*****78</t>
+          <t>(018)-*****43</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1532,22 +1558,22 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>c****0@example.com</t>
+          <t>c*************n@example.net</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>K******n</t>
+          <t>P****g</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>Critical</t>
+          <t>Under Observation</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>70-79</t>
+          <t>90-99</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -1562,43 +1588,45 @@
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>13000-13999</t>
-        </is>
-      </c>
-      <c r="N15" t="n">
-        <v>9296</v>
+          <t>2000-2999</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>*****</t>
+        </is>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Also her stuff job.</t>
+          <t>*****</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>S***t P***y</t>
+          <t>K**e B****s</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>7************7</t>
+          <t>4************7</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>30/04/1974</t>
+          <t>23/09/2002</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>* Turner Turnpike Suite *
-Murphyview, IA *</t>
+          <t>* Cain Camp Suite *
+Ryanbury, MD *</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>(019)-*****52</t>
+          <t>(012)-*****78</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1608,17 +1636,17 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>s*******0@example.net</t>
+          <t>s*******e@example.net</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>M*****a</t>
+          <t>K******n</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>Critical</t>
+          <t>Under Observation</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
@@ -1638,43 +1666,45 @@
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>6000-6999</t>
-        </is>
-      </c>
-      <c r="N16" t="n">
-        <v>8620</v>
+          <t>13000-13999</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>*****</t>
+        </is>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>Center final gun.</t>
+          <t>*****</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>P****a J*****n</t>
+          <t>R***y H****n</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>0************5</t>
+          <t>0************4</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>21/09/1993</t>
+          <t>02/12/1999</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>* Angela Mount
-West Carltown, RI *</t>
+          <t>* John Station
+Granttown, MA *</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>(010)-*****70</t>
+          <t>(012)-*****44</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1684,22 +1714,22 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>a******4@example.org</t>
+          <t>p****s@example.org</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>S***h</t>
+          <t>K******n</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>Recovering</t>
+          <t>Critical</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>30-39</t>
+          <t>50-59</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -1717,40 +1747,42 @@
           <t>8000-8999</t>
         </is>
       </c>
-      <c r="N17" t="n">
-        <v>2213</v>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>*****</t>
+        </is>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>Actually guess let.</t>
+          <t>*****</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>M****n R***n</t>
+          <t>E****d L***z</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>8************0</t>
+          <t>5************8</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>26/07/1957</t>
+          <t>09/12/1981</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>* Ellison Stream
-Angelafurt, PR *</t>
+          <t>* Ward Cliff
+Lake Amanda, FM *</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>(018)-*****64</t>
+          <t>(011)-*****70</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1760,12 +1792,12 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>r*********s@example.com</t>
+          <t>k************n@example.org</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>K**********r</t>
+          <t>S*****k</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -1775,7 +1807,7 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>40-49</t>
+          <t>90-99</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
@@ -1790,43 +1822,45 @@
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>13000-13999</t>
-        </is>
-      </c>
-      <c r="N18" t="n">
-        <v>4920</v>
+          <t>11000-11999</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>*****</t>
+        </is>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Others authority.</t>
+          <t>*****</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>A***r H**l</t>
+          <t>L***s D***s **</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>0************7</t>
+          <t>2************3</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>23/02/1947</t>
+          <t>28/10/1999</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>* Bell Unions Suite *
-Bryanchester, OK *</t>
+          <t>* Ortega Manors Apt. *
+Kennedyton, IL *</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>(010)-*****24</t>
+          <t>(014)-*****67</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1836,22 +1870,22 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>h******c@example.net</t>
+          <t>k*******l@example.net</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>S*****k</t>
+          <t>P****g</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>Recovering</t>
+          <t>Under Observation</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>40-49</t>
+          <t>18-19</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
@@ -1866,43 +1900,45 @@
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>9000-9999</t>
-        </is>
-      </c>
-      <c r="N19" t="n">
-        <v>1451</v>
+          <t>7000-7999</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>*****</t>
+        </is>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Town material.</t>
+          <t>*****</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>F***k H*******n</t>
+          <t>E*******h W**e **</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2************3</t>
+          <t>0************4</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>15/09/1997</t>
+          <t>29/03/1984</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>* Margaret Trafficway
-Alexanderchester, PR *</t>
+          <t>* Albert Hills
+East Charlesfurt, MA *</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>(014)-*****75</t>
+          <t>(014)-*****56</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1912,7 +1948,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>z****e@example.net</t>
+          <t>c***************r@example.com</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -1927,7 +1963,7 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>80-89</t>
+          <t>90-99</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
@@ -1942,43 +1978,45 @@
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>12000-12999</t>
-        </is>
-      </c>
-      <c r="N20" t="n">
-        <v>6623</v>
+          <t>3000-3999</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>*****</t>
+        </is>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Drug head finally.</t>
+          <t>*****</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>K******y S*****n</t>
+          <t>P****a G*****r</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>3************1</t>
+          <t>2************2</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>24/05/1965</t>
+          <t>17/04/1938</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>* Isaac Mountain Apt. *
-Port Jasonchester, FM *</t>
+          <t>* Gould Station
+Mirandabury, UT *</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>(010)-*****15</t>
+          <t>(018)-*****51</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1988,12 +2026,12 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>i*****t@example.org</t>
+          <t>c***********y@example.org</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>P****g</t>
+          <t>S***h</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -2003,7 +2041,7 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>60-69</t>
+          <t>40-49</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
@@ -2018,43 +2056,45 @@
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>6000-6999</t>
-        </is>
-      </c>
-      <c r="N21" t="n">
-        <v>4124</v>
+          <t>4000-4999</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>*****</t>
+        </is>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>National single.</t>
+          <t>*****</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>M****l S*****s</t>
+          <t>M***y A***n</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>4************6</t>
+          <t>8************6</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>23/05/1984</t>
+          <t>02/02/1965</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>* Sara Ranch
-New Christopherfort, MO *</t>
+          <t>* *
+FPO AA *</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>(012)-*****69</t>
+          <t>(017)-*****55</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2064,22 +2104,22 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>s***********a@example.net</t>
+          <t>p**********y@example.net</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>J****************m</t>
+          <t>K******n</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>Critical</t>
+          <t>Healthy</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>90-99</t>
+          <t>50-59</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
@@ -2094,43 +2134,45 @@
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>6000-6999</t>
-        </is>
-      </c>
-      <c r="N22" t="n">
-        <v>8217</v>
+          <t>3000-3999</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>*****</t>
+        </is>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Week woman hear.</t>
+          <t>*****</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>B******y R*******z</t>
+          <t>C*********r W****r</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>6************0</t>
+          <t>6************5</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>12/01/1988</t>
+          <t>02/11/1927</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>* Penny Course Apt. *
-Mckenzieburgh, MA *</t>
+          <t>* Richardson Stravenue
+North Kimberlytown, CA *</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>(017)-*****65</t>
+          <t>(014)-*****90</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2140,12 +2182,12 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>i*******n@example.net</t>
+          <t>m****e@example.org</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>K******n</t>
+          <t>K***h</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -2155,7 +2197,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>100-100</t>
+          <t>50-59</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -2170,43 +2212,45 @@
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>9000-9999</t>
-        </is>
-      </c>
-      <c r="N23" t="n">
-        <v>3753</v>
+          <t>12000-12999</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>*****</t>
+        </is>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Parent chance since.</t>
+          <t>*****</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>S****y F********d</t>
+          <t>S***h A******n</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>9************7</t>
+          <t>4************2</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>28/05/1974</t>
+          <t>06/07/1949</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>* Huang Club Suite *
-West Michael, VI *</t>
+          <t>* *
+FPO AP *</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>(013)-*****43</t>
+          <t>(016)-*****69</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2216,7 +2260,7 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>d********t@example.com</t>
+          <t>b*****b@example.org</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -2226,12 +2270,12 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>Healthy</t>
+          <t>Recovering</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>60-69</t>
+          <t>80-89</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
@@ -2246,43 +2290,45 @@
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>7000-7999</t>
-        </is>
-      </c>
-      <c r="N24" t="n">
-        <v>2508</v>
+          <t>5000-5999</t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>*****</t>
+        </is>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Position few relate.</t>
+          <t>*****</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>P***y D***s</t>
+          <t>A**m T****r</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>0************7</t>
+          <t>5************5</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>15/03/1995</t>
+          <t>26/04/1996</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>* Kelsey Overpass
-Port Deborahmouth, HI *</t>
+          <t>* George Path Apt. *
+Brianhaven, NH *</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>(018)-*****90</t>
+          <t>(011)-*****65</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2292,22 +2338,22 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>n**************s@example.com</t>
+          <t>n*****r@example.com</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>M*****a</t>
+          <t>N*************n</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>Recovering</t>
+          <t>Critical</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>30-39</t>
+          <t>90-99</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
@@ -2322,43 +2368,45 @@
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>14000-14999</t>
-        </is>
-      </c>
-      <c r="N25" t="n">
-        <v>8866</v>
+          <t>13000-13999</t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>*****</t>
+        </is>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Unit political may.</t>
+          <t>*****</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>J**e W******s</t>
+          <t>M*****l A***n</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>6************6</t>
+          <t>4************4</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>06/06/1948</t>
+          <t>20/02/1975</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>* Mcgee Shoals
-Brandiland, IL *</t>
+          <t>* Sanders Tunnel
+New Mia, MA *</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>(016)-*****13</t>
+          <t>(011)-*****93</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2368,12 +2416,12 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>e******z@example.org</t>
+          <t>b*******s@example.com</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>N*************n</t>
+          <t>P***k</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -2383,7 +2431,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>70-79</t>
+          <t>30-39</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -2398,43 +2446,45 @@
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>5000-5999</t>
-        </is>
-      </c>
-      <c r="N26" t="n">
-        <v>7365</v>
+          <t>10000-10999</t>
+        </is>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>*****</t>
+        </is>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Will early her.</t>
+          <t>*****</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>A**m W******s</t>
+          <t>C*****l S***e</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>7************5</t>
+          <t>2************0</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>30/08/1983</t>
+          <t>10/11/1928</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>* Brown Ramp
-East Joe, OK *</t>
+          <t>* Mindy Ramp Apt. *
+Stuartfort, WY *</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>(016)-*****03</t>
+          <t>(012)-*****96</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2444,22 +2494,22 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>t**********r@example.net</t>
+          <t>j**********s@example.com</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>P****s</t>
+          <t>S*****k</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>Critical</t>
+          <t>Needs Attention</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>20-29</t>
+          <t>40-49</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
@@ -2474,43 +2524,45 @@
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>11000-11999</t>
-        </is>
-      </c>
-      <c r="N27" t="n">
-        <v>2025</v>
+          <t>10000-10999</t>
+        </is>
+      </c>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>*****</t>
+        </is>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>You company window.</t>
+          <t>*****</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>K***a M****n</t>
+          <t>J**n P**k</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>0************3</t>
+          <t>8************0</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>31/05/1968</t>
+          <t>03/06/1925</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>* Jeremy Fall
-Taraton, WA *</t>
+          <t>* Franco Burg
+Gonzalezbury, OK *</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>(010)-*****34</t>
+          <t>(011)-*****71</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2520,22 +2572,22 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>a****5@example.com</t>
+          <t>a****8@example.org</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>S******r</t>
+          <t>P****s</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>Under Observation</t>
+          <t>Critical</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>30-39</t>
+          <t>50-59</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
@@ -2550,43 +2602,45 @@
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>6000-6999</t>
-        </is>
-      </c>
-      <c r="N28" t="n">
-        <v>2408</v>
+          <t>2000-2999</t>
+        </is>
+      </c>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>*****</t>
+        </is>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Hold job similar.</t>
+          <t>*****</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>M*****l R*******z</t>
+          <t>G**e S***h</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>5************5</t>
+          <t>4************7</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>26/01/1973</t>
+          <t>22/04/1994</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>* Travis Court
-Markport, IL *</t>
+          <t>* Brian Union Apt. *
+Lake Carolynton, IA *</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>(012)-*****77</t>
+          <t>(012)-*****84</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2596,7 +2650,7 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>e********y@example.net</t>
+          <t>q******z@example.com</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
@@ -2606,12 +2660,12 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>Under Observation</t>
+          <t>Needs Attention</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>18-19</t>
+          <t>30-39</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
@@ -2626,43 +2680,45 @@
       </c>
       <c r="M29" t="inlineStr">
         <is>
-          <t>5000-5999</t>
-        </is>
-      </c>
-      <c r="N29" t="n">
-        <v>6232</v>
+          <t>4000-4999</t>
+        </is>
+      </c>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>*****</t>
+        </is>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Interesting visit.</t>
+          <t>*****</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>K***n B*****n</t>
+          <t>A*****l S*****z</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>0************8</t>
+          <t>3************4</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>12/01/1968</t>
+          <t>19/12/1965</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>* Samantha Canyon
-Mortonstad, MT *</t>
+          <t>Unit * Box *
+DPO AP *</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>(015)-*****28</t>
+          <t>(010)-*****49</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2672,22 +2728,22 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>s*******6@example.com</t>
+          <t>s****n@example.org</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>M*****a</t>
+          <t>J****************m</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>Critical</t>
+          <t>Recovering</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>80-89</t>
+          <t>30-39</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
@@ -2702,43 +2758,45 @@
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>2000-2999</t>
-        </is>
-      </c>
-      <c r="N30" t="n">
-        <v>4306</v>
+          <t>4000-4999</t>
+        </is>
+      </c>
+      <c r="N30" t="inlineStr">
+        <is>
+          <t>*****</t>
+        </is>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>West reach.</t>
+          <t>*****</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>P**l P***z</t>
+          <t>M******e G****a</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>6************7</t>
+          <t>0************4</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>28/12/1960</t>
+          <t>22/09/1958</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>* Heather Meadows Apt. *
-Henryville, SD *</t>
+          <t>* Robin Falls
+Leeburgh, IL *</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>(013)-*****04</t>
+          <t>(010)-*****24</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2748,22 +2806,22 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>a******5@example.com</t>
+          <t>m***********s@example.org</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>S***h</t>
+          <t>K******n</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>Healthy</t>
+          <t>Recovering</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>30-39</t>
+          <t>20-29</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
@@ -2781,12 +2839,14 @@
           <t>9000-9999</t>
         </is>
       </c>
-      <c r="N31" t="n">
-        <v>5769</v>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>*****</t>
+        </is>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Team artist fire.</t>
+          <t>*****</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Finalized the main functions
</commit_message>
<xml_diff>
--- a/backend/uploads/masked/masked_Student_Information.xlsx
+++ b/backend/uploads/masked/masked_Student_Information.xlsx
@@ -513,28 +513,28 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>C******y B***n</t>
+          <t>K****y H***s</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0************9</t>
+          <t>2************4</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>12/07/1989</t>
+          <t>03/02/2006</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Unit * Box *
-DPO AE *</t>
+          <t>* Elizabeth Wells
+Port Samantha, AR *</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>(016)-*****95</t>
+          <t>(018)-*****14</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -544,22 +544,22 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>l********e@example.org</t>
+          <t>d********0@example.com</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>P****g</t>
+          <t>P***k</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Critical</t>
+          <t>Needs Attention</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>60-69</t>
+          <t>50-59</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -574,7 +574,7 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>12000-12999</t>
+          <t>3000-3999</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
@@ -591,28 +591,28 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>G*****y M****n J*.</t>
+          <t>G*****l D**e **</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>4************0</t>
+          <t>7************7</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>26/10/2006</t>
+          <t>24/01/1967</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>* Johnson Square Suite *
-Burkeburgh, TX *</t>
+          <t>* David Highway Suite *
+East Daniel, KY *</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>(015)-*****35</t>
+          <t>(016)-*****76</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -622,22 +622,22 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>e*********2@example.org</t>
+          <t>n********1@example.org</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>P***k</t>
+          <t>T********u</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Healthy</t>
+          <t>Critical</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>30-39</t>
+          <t>90-99</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -652,7 +652,7 @@
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>4000-4999</t>
+          <t>8000-8999</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
@@ -669,28 +669,28 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>F*******k S**o</t>
+          <t>T***r F********d</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>6************3</t>
+          <t>2************8</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>18/09/1933</t>
+          <t>03/11/1978</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>* Evan Parkways Suite *
-New Kenneth, MS *</t>
+          <t>* Dickerson Inlet
+Port Melissa, AL *</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>(016)-*****16</t>
+          <t>(016)-*****31</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -700,12 +700,12 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>b********0@example.net</t>
+          <t>c*********n@example.net</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>K***h</t>
+          <t>J****************m</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -715,7 +715,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>100-100</t>
+          <t>40-49</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -730,7 +730,7 @@
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>3000-3999</t>
+          <t>7000-7999</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
@@ -747,28 +747,28 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>J***n B***y</t>
+          <t>M*****l H****s</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>5************9</t>
+          <t>8************0</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>16/12/1945</t>
+          <t>27/10/1982</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>* Frank Expressway
-West Evanfurt, GA *</t>
+          <t>* Perez Track
+Curryview, FL *</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>(011)-*****12</t>
+          <t>(016)-*****79</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -778,22 +778,22 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>k*********s@example.com</t>
+          <t>h************o@example.com</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>K***h</t>
+          <t>P****s</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Under Observation</t>
+          <t>Recovering</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>70-79</t>
+          <t>20-29</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -808,7 +808,7 @@
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>4000-4999</t>
+          <t>6000-6999</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
@@ -825,28 +825,28 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>R**n M***y</t>
+          <t>S***n T****s</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>3************0</t>
+          <t>5************3</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>11/02/1971</t>
+          <t>12/04/1976</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>* Gilmore Lake Suite *
-Snyderland, WA *</t>
+          <t>* Alan Walk Suite *
+New Cristianshire, PR *</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>(018)-*****39</t>
+          <t>(019)-*****26</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -856,22 +856,22 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>o*********e@example.net</t>
+          <t>v*****r@example.com</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>P***k</t>
+          <t>S*****k</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Needs Attention</t>
+          <t>Recovering</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>20-29</t>
+          <t>18-19</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -886,7 +886,7 @@
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>5000-5999</t>
+          <t>14000-14999</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
@@ -903,28 +903,28 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>A***r P**a</t>
+          <t>O****a **</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>9************1</t>
+          <t>8************8</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>13/03/1999</t>
+          <t>09/05/1962</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>* Travis Ways Apt. *
-Smithstad, MH *</t>
+          <t>* Melton Junction
+Zacharyport, KS *</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>(013)-*****72</t>
+          <t>(014)-*****11</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -934,12 +934,12 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>s***********w@example.net</t>
+          <t>j********3@example.com</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>K***h</t>
+          <t>P***k</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -964,7 +964,7 @@
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>5000-5999</t>
+          <t>14000-14999</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
@@ -981,7 +981,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>E****d L********n</t>
+          <t>A*n H*******s</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -991,18 +991,18 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>30/11/1977</t>
+          <t>30/08/1965</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>* Doyle Bypass Suite *
-Valerieville, CA *</t>
+          <t>* Byrd Expressway Suite *
+East John, TX *</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>(017)-*****65</t>
+          <t>(017)-*****11</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1012,22 +1012,22 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>l******s@example.com</t>
+          <t>j**********p@example.net</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>P****g</t>
+          <t>S******r</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Under Observation</t>
+          <t>Critical</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>20-29</t>
+          <t>80-89</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
@@ -1042,7 +1042,7 @@
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>6000-6999</t>
+          <t>10000-10999</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
@@ -1059,28 +1059,28 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>M****s C*x</t>
+          <t>B*****y M*******o</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>8************6</t>
+          <t>8************4</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>01/02/1924</t>
+          <t>13/10/1972</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>* Skinner Street
-East Katherineville, MA *</t>
+          <t>* Chad Lodge
+Port Suzanneview, AZ *</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>(015)-*****09</t>
+          <t>(018)-*****94</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1090,22 +1090,22 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>e******l@example.org</t>
+          <t>h*****r@example.org</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>S***h</t>
+          <t>K**********r</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Needs Attention</t>
+          <t>Recovering</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>80-89</t>
+          <t>50-59</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -1120,7 +1120,7 @@
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>12000-12999</t>
+          <t>2000-2999</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
@@ -1137,28 +1137,28 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>M*****l A******n</t>
+          <t>V****r A***n</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>8************7</t>
+          <t>6************0</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>02/12/1981</t>
+          <t>12/02/2004</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>* Bell Causeway
-Lake Jamesborough, OH *</t>
+          <t>* Bennett Junctions Suite *
+Farrellmouth, FM *</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>(013)-*****60</t>
+          <t>(017)-*****04</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1168,12 +1168,12 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>j************t@example.com</t>
+          <t>p****4@example.net</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>M*****a</t>
+          <t>K**********r</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -1183,7 +1183,7 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>80-89</t>
+          <t>40-49</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
@@ -1198,7 +1198,7 @@
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>9000-9999</t>
+          <t>4000-4999</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
@@ -1215,7 +1215,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>D****e R*****z</t>
+          <t>A*******a S*****r</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1225,18 +1225,18 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>19/12/1985</t>
+          <t>14/12/1996</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Unit * Box *
-DPO AA *</t>
+          <t>* *
+FPO AP *</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>(012)-*****82</t>
+          <t>(019)-*****04</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1246,17 +1246,17 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>c*******6@example.com</t>
+          <t>l*******n@example.net</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>P****g</t>
+          <t>S***h</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Recovering</t>
+          <t>Needs Attention</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
@@ -1276,7 +1276,7 @@
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>11000-11999</t>
+          <t>12000-12999</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
@@ -1293,7 +1293,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>J****a C***k J*.</t>
+          <t>D**n W***s</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1303,18 +1303,18 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>08/04/1961</t>
+          <t>10/09/1947</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>* Walker Locks Suite *
-West Josephview, MH *</t>
+          <t>* Kelly Coves Apt. *
+New Richard, PR *</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>(016)-*****73</t>
+          <t>(019)-*****46</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1324,22 +1324,22 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>k************s@example.org</t>
+          <t>j**********r@example.org</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>S******r</t>
+          <t>M*****a</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>Under Observation</t>
+          <t>Needs Attention</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>50-59</t>
+          <t>80-89</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
@@ -1354,7 +1354,7 @@
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>4000-4999</t>
+          <t>7000-7999</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
@@ -1371,28 +1371,28 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>R*****o K***y</t>
+          <t>J**n W******s</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>0************2</t>
+          <t>7************4</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>05/03/2006</t>
+          <t>03/07/1959</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>* Jessica Spurs Apt. *
-Reneeland, SC *</t>
+          <t>* Soto Walks Apt. *
+Simsbury, AR *</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>(015)-*****16</t>
+          <t>(010)-*****24</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1402,12 +1402,12 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>m********n@example.org</t>
+          <t>b*************n@example.net</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>S******r</t>
+          <t>P****s</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -1417,7 +1417,7 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>50-59</t>
+          <t>80-89</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
@@ -1432,7 +1432,7 @@
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>3000-3999</t>
+          <t>10000-10999</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
@@ -1449,28 +1449,28 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>M*. W*****m P*****s</t>
+          <t>S*****n S*******r</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>5************7</t>
+          <t>0************6</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>23/12/1929</t>
+          <t>07/01/1944</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>* Holly Bypass
-Port Katherinechester, TN *</t>
+          <t>* Patrick Islands Apt. *
+Lake Joshuaside, NC *</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>(016)-*****86</t>
+          <t>(014)-*****19</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1480,22 +1480,22 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>n***l@example.org</t>
+          <t>p*******l@example.org</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>N*************n</t>
+          <t>K**********r</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>Needs Attention</t>
+          <t>Recovering</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>40-49</t>
+          <t>50-59</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -1510,7 +1510,7 @@
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>7000-7999</t>
+          <t>2000-2999</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
@@ -1527,28 +1527,28 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>T****s H*******z</t>
+          <t>C*********r T****s</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>6************4</t>
+          <t>4************4</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>02/07/1988</t>
+          <t>27/02/1967</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>* Carr Run
-Hillton, PA *</t>
+          <t>* Christina Overpass
+Robinsontown, PR *</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>(013)-*****28</t>
+          <t>(015)-*****98</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1558,22 +1558,22 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>h*****l@example.org</t>
+          <t>c*******3@example.org</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>P****s</t>
+          <t>P***k</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>Critical</t>
+          <t>Recovering</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>20-29</t>
+          <t>80-89</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -1588,7 +1588,7 @@
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>9000-9999</t>
+          <t>7000-7999</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
@@ -1605,28 +1605,28 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>J*****e W*******n</t>
+          <t>J****e C***y</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>9************0</t>
+          <t>3************7</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>20/07/1933</t>
+          <t>09/11/1992</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>* Green Key
-New Tammy, DE *</t>
+          <t>* Keller Plains Suite *
+North Nicolehaven, NC *</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>(011)-*****97</t>
+          <t>(019)-*****65</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1636,22 +1636,22 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>q*****n@example.org</t>
+          <t>k*********e@example.com</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>S***h</t>
+          <t>T********u</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>Healthy</t>
+          <t>Recovering</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>40-49</t>
+          <t>50-59</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
@@ -1666,7 +1666,7 @@
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>9000-9999</t>
+          <t>3000-3999</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
@@ -1683,28 +1683,28 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>J******r M****a</t>
+          <t>K*m W****n</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>3************2</t>
+          <t>2************5</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>21/02/2001</t>
+          <t>06/02/1946</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>* Sarah Center Suite *
-Port Victoriaville, MD *</t>
+          <t>* Anna Creek Apt. *
+North Jessica, VA *</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>(011)-*****45</t>
+          <t>(019)-*****08</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1714,12 +1714,12 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>l******n@example.net</t>
+          <t>p*******n@example.org</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>M*****a</t>
+          <t>P****g</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -1729,7 +1729,7 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>80-89</t>
+          <t>70-79</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -1744,7 +1744,7 @@
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>10000-10999</t>
+          <t>6000-6999</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
@@ -1761,7 +1761,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>J***s W***s</t>
+          <t>L**a B****s D*S</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1771,18 +1771,18 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>05/01/1928</t>
+          <t>28/05/1955</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>* Garcia Village
-Garciafurt, ND *</t>
+          <t>* Tina Parkway Apt. *
+South Francismouth, SD *</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>(015)-*****60</t>
+          <t>(017)-*****28</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1792,12 +1792,12 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>b*****5@example.com</t>
+          <t>e****6@example.org</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>P****g</t>
+          <t>P***k</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -1807,7 +1807,7 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>20-29</t>
+          <t>70-79</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
@@ -1822,7 +1822,7 @@
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>8000-8999</t>
+          <t>13000-13999</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
@@ -1839,28 +1839,28 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>M**s N*****a H****s D*S</t>
+          <t>M**y M***n</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>4************1</t>
+          <t>9************5</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>01/11/1972</t>
+          <t>25/11/1960</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>* Bauer Skyway Apt. *
-South Davidport, NE *</t>
+          <t>* Elizabeth Fields Suite *
+Douglasberg, RI *</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>(011)-*****11</t>
+          <t>(019)-*****51</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1870,12 +1870,12 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>c**********l@example.net</t>
+          <t>p***********l@example.net</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>P****s</t>
+          <t>S******r</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -1885,7 +1885,7 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>80-89</t>
+          <t>30-39</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
@@ -1900,7 +1900,7 @@
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>2000-2999</t>
+          <t>10000-10999</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
@@ -1917,28 +1917,28 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>M*****l M****n</t>
+          <t>K***e G***n</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>5************5</t>
+          <t>9************3</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>02/05/1951</t>
+          <t>12/11/1975</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>* Brooks Crest Suite *
-Malonechester, OR *</t>
+          <t>* Courtney Roads Suite *
+North Jerrychester, OR *</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>(017)-*****61</t>
+          <t>(018)-*****89</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1948,12 +1948,12 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>j*******n@example.org</t>
+          <t>t********a@example.org</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>N*************n</t>
+          <t>S***h</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -1963,7 +1963,7 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>20-29</t>
+          <t>60-69</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
@@ -1978,7 +1978,7 @@
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>10000-10999</t>
+          <t>14000-14999</t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
@@ -1995,28 +1995,28 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>L****e P****r</t>
+          <t>E****d L**g</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2************2</t>
+          <t>4************1</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>01/09/1974</t>
+          <t>12/07/1949</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>* Yvonne Estate Suite *
-Lake Kevinton, DC *</t>
+          <t>* Patterson Circle
+West Dawnville, CA *</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>(015)-*****70</t>
+          <t>(014)-*****45</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2026,22 +2026,22 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>r*********a@example.org</t>
+          <t>a******s@example.org</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>S***h</t>
+          <t>K***h</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>Needs Attention</t>
+          <t>Critical</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>40-49</t>
+          <t>50-59</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
@@ -2056,7 +2056,7 @@
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>9000-9999</t>
+          <t>14000-14999</t>
         </is>
       </c>
       <c r="N21" t="inlineStr">
@@ -2073,28 +2073,28 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>M**y D***s</t>
+          <t>J**l F******n</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>9************6</t>
+          <t>0************3</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>03/04/1924</t>
+          <t>15/02/1933</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>* Vazquez Mountain
-North Karenstad, GU *</t>
+          <t>* Megan Camp
+East Davidbury, ND *</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>(010)-*****76</t>
+          <t>(017)-*****16</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2104,22 +2104,22 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>h*********l@example.com</t>
+          <t>a*******8@example.org</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>P****g</t>
+          <t>P***k</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>Needs Attention</t>
+          <t>Critical</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>30-39</t>
+          <t>60-69</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
@@ -2134,7 +2134,7 @@
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>11000-11999</t>
+          <t>14000-14999</t>
         </is>
       </c>
       <c r="N22" t="inlineStr">
@@ -2151,28 +2151,28 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>N****n H****s</t>
+          <t>K******n H***s</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>0************4</t>
+          <t>8************6</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>20/04/1970</t>
+          <t>29/07/1956</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>* Karen Freeway
-Lopezville, NH *</t>
+          <t>* *
+FPO AA *</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>(012)-*****92</t>
+          <t>(019)-*****83</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2182,7 +2182,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>b*********n@example.org</t>
+          <t>f***********w@example.org</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -2192,12 +2192,12 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>Under Observation</t>
+          <t>Healthy</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>90-99</t>
+          <t>60-69</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -2212,7 +2212,7 @@
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>13000-13999</t>
+          <t>10000-10999</t>
         </is>
       </c>
       <c r="N23" t="inlineStr">
@@ -2229,28 +2229,28 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>C*****a D****y</t>
+          <t>S******a R*******z</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>8************8</t>
+          <t>3************7</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>26/06/1949</t>
+          <t>10/05/1977</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>* Gordon Extension Apt. *
-West Kimberlyfort, MP *</t>
+          <t>* Dustin Fork
+West Katietown, MH *</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>(018)-*****72</t>
+          <t>(019)-*****65</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2260,12 +2260,12 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>f****z@example.org</t>
+          <t>h******0@example.com</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>S*****k</t>
+          <t>K******n</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
@@ -2275,7 +2275,7 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>20-29</t>
+          <t>60-69</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
@@ -2290,7 +2290,7 @@
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>2000-2999</t>
+          <t>5000-5999</t>
         </is>
       </c>
       <c r="N24" t="inlineStr">
@@ -2307,28 +2307,28 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>M***n G**y</t>
+          <t>J******r R*****d</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>4************7</t>
+          <t>8************7</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>12/06/1972</t>
+          <t>12/04/1944</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>* Dale Valley
-North Kellistad, RI *</t>
+          <t>* Vasquez Ford
+West Alexshire, NH *</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>(015)-*****73</t>
+          <t>(013)-*****79</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2338,22 +2338,22 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>d*****s@example.org</t>
+          <t>r********z@example.net</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>P***k</t>
+          <t>K******n</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>Critical</t>
+          <t>Recovering</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>40-49</t>
+          <t>60-69</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
@@ -2368,7 +2368,7 @@
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>10000-10999</t>
+          <t>13000-13999</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
@@ -2385,28 +2385,28 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>R****y Y***g</t>
+          <t>D******e S****r</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>2************3</t>
+          <t>8************1</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>28/05/1934</t>
+          <t>09/05/1962</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>* Martin Trafficway
-New Nicole, KY *</t>
+          <t>* Matthew Squares Apt. *
+East Shawnville, TX *</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>(011)-*****26</t>
+          <t>(011)-*****52</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2416,7 +2416,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>h*i@example.org</t>
+          <t>i****d@example.com</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -2431,7 +2431,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>30-39</t>
+          <t>70-79</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -2446,7 +2446,7 @@
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>9000-9999</t>
+          <t>14000-14999</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
@@ -2463,28 +2463,28 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>J***s T**e</t>
+          <t>T*****y H*******z</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>5************6</t>
+          <t>9************3</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>28/04/1993</t>
+          <t>10/04/1971</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>* Christina Groves
-Williambury, AS *</t>
+          <t>* Lewis Rapids Suite *
+Lake Gregoryfurt, AS *</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>(017)-*****76</t>
+          <t>(019)-*****05</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2494,22 +2494,22 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>w*******0@example.org</t>
+          <t>y***g@example.net</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>S******r</t>
+          <t>T********u</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>Recovering</t>
+          <t>Needs Attention</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>20-29</t>
+          <t>30-39</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
@@ -2524,7 +2524,7 @@
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>13000-13999</t>
+          <t>3000-3999</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
@@ -2541,28 +2541,28 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>M****a B****s</t>
+          <t>K****a N****s</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>0************0</t>
+          <t>8************3</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>28/01/1990</t>
+          <t>03/09/1983</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>* Brenda Mountain
-Johnberg, MH *</t>
+          <t>* Isaac Ports
+East Angela, GA *</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>(013)-*****97</t>
+          <t>(011)-*****65</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2572,22 +2572,22 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>x********z@example.org</t>
+          <t>v*********y@example.org</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>S*****k</t>
+          <t>T********u</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>Critical</t>
+          <t>Healthy</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>30-39</t>
+          <t>50-59</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
@@ -2619,28 +2619,28 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>J***s B****n</t>
+          <t>R*****d F***z</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>4************6</t>
+          <t>6************0</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>12/05/2003</t>
+          <t>01/07/1988</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>* Maria Union
-East Gerald, NY *</t>
+          <t>* Joshua Roads Apt. *
+New Duane, KS *</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>(018)-*****85</t>
+          <t>(013)-*****26</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2650,12 +2650,12 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>b*********y@example.net</t>
+          <t>a***8@example.org</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>T********u</t>
+          <t>K**********r</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -2665,7 +2665,7 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>60-69</t>
+          <t>50-59</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
@@ -2697,28 +2697,28 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>M*****l H**s</t>
+          <t>P****a T****r</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>4************0</t>
+          <t>7************0</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>22/10/1983</t>
+          <t>09/08/1962</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>* Morgan Ramp Apt. *
-Kruegerfort, MH *</t>
+          <t>* Gonzalez Way
+New Jared, NY *</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>(016)-*****62</t>
+          <t>(018)-*****52</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2728,22 +2728,22 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>w******t@example.org</t>
+          <t>s******5@example.com</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>K**********r</t>
+          <t>T********u</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>Critical</t>
+          <t>Recovering</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>90-99</t>
+          <t>20-29</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
@@ -2758,7 +2758,7 @@
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>4000-4999</t>
+          <t>12000-12999</t>
         </is>
       </c>
       <c r="N30" t="inlineStr">
@@ -2775,28 +2775,28 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>K***n B****n</t>
+          <t>T***y L***s</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>4************4</t>
+          <t>3************3</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>08/06/1963</t>
+          <t>09/01/1976</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>* Brandy Valleys Suite *
-Evanborough, ND *</t>
+          <t>* Coleman Mission
+Doyleborough, DE *</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>(018)-*****53</t>
+          <t>(011)-*****49</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2806,22 +2806,22 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>l****5@example.net</t>
+          <t>k********7@example.com</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>S*****k</t>
+          <t>K***h</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>Healthy</t>
+          <t>Needs Attention</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>70-79</t>
+          <t>80-89</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
@@ -2836,7 +2836,7 @@
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>10000-10999</t>
+          <t>3000-3999</t>
         </is>
       </c>
       <c r="N31" t="inlineStr">

</xml_diff>